<commit_message>
Update templates, format with Ruff, remove old notebooks
</commit_message>
<xml_diff>
--- a/templates/Experimental_Analyses_Template.xlsx
+++ b/templates/Experimental_Analyses_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmith/LEPR_traceDs/Templates/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985513E5-8D33-324D-BF59-02C1FA313B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39855223-A51F-504C-BE89-F979E5736520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30340" yWindow="1580" windowWidth="38700" windowHeight="23680" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61860" yWindow="15000" windowWidth="28460" windowHeight="20420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data Source" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="183">
   <si>
     <t>Measured Parameter</t>
   </si>
@@ -476,9 +476,6 @@
   </si>
   <si>
     <t>must match a code in the DATA tab (or one of the BULK tabs) row 3</t>
-  </si>
-  <si>
-    <t>must match a parameter in the DATA tab (or one fo the BULK tabs) row 2</t>
   </si>
   <si>
     <t>assign a number that links method to paramater(s); must match the DATA tab (or one of the BULK tabs) row 3</t>
@@ -588,13 +585,16 @@
     <t>LEPR (only) or traceDs</t>
   </si>
   <si>
-    <t>PHASES [list]</t>
-  </si>
-  <si>
     <t>Starting Material Information</t>
   </si>
   <si>
     <t>Run Products Information</t>
+  </si>
+  <si>
+    <t>PARAMETER (or PHASE) [list]</t>
+  </si>
+  <si>
+    <t>PHASE (or PARAMETER) [list]</t>
   </si>
   <si>
     <r>
@@ -609,7 +609,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>PHASES list</t>
+      <t>PHASE list</t>
     </r>
     <r>
       <rPr>
@@ -630,6 +630,9 @@
       </rPr>
       <t>in column F onwards</t>
     </r>
+  </si>
+  <si>
+    <t>must match a parameter in the DATA tab (or one of the BULK tabs) row 2</t>
   </si>
 </sst>
 </file>
@@ -2385,7 +2388,7 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2511,7 +2514,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E5" s="41" t="s">
         <v>53</v>
@@ -2606,7 +2609,7 @@
   <dimension ref="A1:BL6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2614,13 +2617,13 @@
     <col min="1" max="1" width="17.33203125" style="139" customWidth="1"/>
     <col min="2" max="5" width="15.6640625" style="139" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" style="139" customWidth="1"/>
-    <col min="7" max="7" width="24" style="139" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="139" customWidth="1"/>
     <col min="8" max="16384" width="10.6640625" style="139"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="133" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="187" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B1" s="187"/>
       <c r="C1" s="187"/>
@@ -2638,7 +2641,7 @@
       <c r="E2" s="134"/>
       <c r="F2" s="134"/>
       <c r="G2" s="128" t="s">
-        <v>54</v>
+        <v>179</v>
       </c>
       <c r="H2" s="135"/>
       <c r="I2" s="135"/>
@@ -2853,7 +2856,7 @@
         <v>136</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E5" s="147" t="s">
         <v>59</v>
@@ -2876,7 +2879,7 @@
         <v>137</v>
       </c>
       <c r="D6" s="148" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6" s="148" t="s">
         <v>138</v>
@@ -2917,13 +2920,13 @@
     <col min="2" max="2" width="19.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="2" customWidth="1"/>
     <col min="6" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="160" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B1" s="160"/>
       <c r="C1" s="162"/>
@@ -2937,7 +2940,7 @@
       <c r="C2" s="105"/>
       <c r="D2" s="105"/>
       <c r="E2" s="128" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -3304,7 +3307,7 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3336,7 +3339,7 @@
   <sheetData>
     <row r="1" spans="1:26" s="24" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="188" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B1" s="188"/>
       <c r="C1" s="125"/>
@@ -3394,14 +3397,14 @@
     </row>
     <row r="3" spans="1:26" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="191" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="192" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="87" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" s="87"/>
       <c r="F3" s="87"/>
@@ -3409,25 +3412,25 @@
       <c r="H3" s="88"/>
       <c r="I3" s="23"/>
       <c r="J3" s="92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K3" s="92"/>
       <c r="L3" s="92"/>
       <c r="M3" s="23"/>
       <c r="N3" s="193" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O3" s="193"/>
       <c r="P3" s="95"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="93" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S3" s="93"/>
       <c r="T3" s="93"/>
       <c r="U3" s="82"/>
       <c r="V3" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W3" s="34"/>
       <c r="X3" s="34"/>
@@ -3436,10 +3439,10 @@
     </row>
     <row r="4" spans="1:26" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="118" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="163" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="64" t="s">
@@ -3452,40 +3455,40 @@
         <v>9</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" s="66" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="172" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="L4" s="77" t="s">
         <v>172</v>
-      </c>
-      <c r="K4" s="77" t="s">
-        <v>174</v>
-      </c>
-      <c r="L4" s="77" t="s">
-        <v>173</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="85" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O4" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="P4" s="85" t="s">
         <v>163</v>
-      </c>
-      <c r="P4" s="85" t="s">
-        <v>164</v>
       </c>
       <c r="Q4" s="17"/>
       <c r="R4" s="78" t="s">
         <v>132</v>
       </c>
       <c r="S4" s="78" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T4" s="78" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U4" s="16"/>
       <c r="V4" s="79"/>
@@ -3496,23 +3499,23 @@
     </row>
     <row r="5" spans="1:26" s="30" customFormat="1" ht="52" x14ac:dyDescent="0.2">
       <c r="A5" s="167" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="167" t="s">
         <v>151</v>
-      </c>
-      <c r="B5" s="167" t="s">
-        <v>152</v>
       </c>
       <c r="C5" s="164"/>
       <c r="D5" s="165" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="165" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F5" s="173" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="165" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>19</v>
@@ -3526,7 +3529,7 @@
         <v>128</v>
       </c>
       <c r="O5" s="169" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P5" s="169" t="s">
         <v>130</v>
@@ -3539,7 +3542,7 @@
         <v>129</v>
       </c>
       <c r="T5" s="173" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U5" s="17"/>
       <c r="V5" s="79"/>
@@ -3641,7 +3644,7 @@
   <dimension ref="A1:BL6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3650,7 +3653,7 @@
     <col min="2" max="2" width="16.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="2" customWidth="1"/>
     <col min="4" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27" style="2" customWidth="1"/>
     <col min="8" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
@@ -4195,10 +4198,10 @@
     </row>
     <row r="5" spans="1:15" s="30" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A5" s="119" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="119" t="s">
         <v>148</v>
-      </c>
-      <c r="B5" s="119" t="s">
-        <v>149</v>
       </c>
       <c r="C5" s="67"/>
       <c r="D5" s="127" t="s">
@@ -4296,7 +4299,7 @@
   <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4441,7 +4444,7 @@
       <c r="AA3" s="95"/>
       <c r="AB3" s="82"/>
       <c r="AC3" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AD3" s="34"/>
       <c r="AE3" s="34"/>
@@ -4530,7 +4533,7 @@
         <v>146</v>
       </c>
       <c r="B5" s="119" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="C5" s="81"/>
       <c r="D5" s="51"/>

</xml_diff>

<commit_message>
Updated with proper DOI: https://ecl.earthchem.org/view.php?id=3570
</commit_message>
<xml_diff>
--- a/templates/Experimental_Analyses_Template.xlsx
+++ b/templates/Experimental_Analyses_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmith/LEPR_traceDs/Templates/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmith/Downloads/Browser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDF4C889-8DF6-8943-9C0C-1DF392F4081C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF8FFE9-8865-1040-8BED-A2256DE08378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30840" yWindow="-12660" windowWidth="32480" windowHeight="19860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31400" yWindow="-800" windowWidth="28820" windowHeight="18040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data Source" sheetId="7" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>Powered by EarthChem</t>
   </si>
   <si>
-    <t>v3.1 last modified 03/23/2022</t>
-  </si>
-  <si>
     <t>INSTRUMENT</t>
   </si>
   <si>
@@ -714,12 +711,6 @@
     <t>optional descripion for  (e.g. 'volatiles', 'mineral', 'glass') or leave blank for all analyses in same batch</t>
   </si>
   <si>
-    <t>10.26022/IEDA/112265</t>
-  </si>
-  <si>
-    <t>Template developed by EarthChem</t>
-  </si>
-  <si>
     <t>experiment</t>
   </si>
   <si>
@@ -790,13 +781,22 @@
   </si>
   <si>
     <t>e.g. WC, sintered diamond, diamond, moissanite</t>
+  </si>
+  <si>
+    <t>v3.0 last modified 11/26/2024</t>
+  </si>
+  <si>
+    <t>Template developed by LEPR - IEDA2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.60520/IEDA/113570</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1072,19 +1072,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1221,12 +1215,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB8CCE4"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1404,7 +1392,7 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1795,9 +1783,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1812,6 +1797,60 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="40" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="13" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1819,14 +1858,15 @@
     <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1834,70 +1874,14 @@
     <xf numFmtId="0" fontId="35" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="13" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="40" fillId="25" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="25" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="25" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="13" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2311,24 +2295,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="32" style="18" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.6640625" style="18" customWidth="1"/>
     <col min="4" max="16384" width="10.6640625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="190" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="196" t="s">
+      <c r="B1" s="191"/>
+      <c r="C1" s="201" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2336,16 +2320,16 @@
       <c r="A2" s="159" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="181" t="s">
-        <v>206</v>
+      <c r="B2" s="159" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="160" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="182" t="s">
-        <v>205</v>
+      <c r="A3" s="202" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="203" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2545,7 +2529,7 @@
       <c r="C31" s="45"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="183" t="s">
+      <c r="A33" s="170" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2563,7 +2547,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B08ECCD3-C2D0-6741-AA7B-4286C6001D63}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{41CFE403-77AC-8049-88BB-3A1B36BA1885}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{6F0BB47F-E6ED-4299-9C87-98C479C75A20}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{636F77BA-E1BD-4DF1-8D23-F141B330D868}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2575,7 +2560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2598,64 +2585,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="194" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="196" t="s">
+      <c r="A1" s="114" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="197"/>
-      <c r="K1" s="197"/>
-      <c r="L1" s="197"/>
-      <c r="M1" s="197"/>
-      <c r="N1" s="197"/>
-      <c r="O1" s="197"/>
-      <c r="P1" s="197"/>
-      <c r="Q1" s="197"/>
-      <c r="R1" s="198"/>
-      <c r="S1" s="198"/>
-      <c r="T1" s="198"/>
-      <c r="U1" s="198"/>
-      <c r="V1" s="198"/>
-      <c r="W1" s="198"/>
-      <c r="X1" s="198"/>
-      <c r="Y1" s="198"/>
-      <c r="Z1" s="198"/>
+      <c r="E1" s="183"/>
+      <c r="F1" s="183"/>
+      <c r="G1" s="183"/>
+      <c r="H1" s="183"/>
+      <c r="I1" s="183"/>
+      <c r="J1" s="183"/>
+      <c r="K1" s="183"/>
+      <c r="L1" s="183"/>
+      <c r="M1" s="183"/>
+      <c r="N1" s="183"/>
+      <c r="O1" s="183"/>
+      <c r="P1" s="183"/>
+      <c r="Q1" s="183"/>
+      <c r="R1" s="183"/>
+      <c r="S1" s="183"/>
+      <c r="T1" s="183"/>
+      <c r="U1" s="183"/>
+      <c r="V1" s="183"/>
+      <c r="W1" s="183"/>
+      <c r="X1" s="183"/>
+      <c r="Y1" s="183"/>
+      <c r="Z1" s="183"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A2" s="197"/>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="197"/>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197"/>
-      <c r="M2" s="197"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="198"/>
-      <c r="S2" s="198"/>
-      <c r="T2" s="198"/>
-      <c r="U2" s="198"/>
-      <c r="V2" s="198"/>
-      <c r="W2" s="198"/>
-      <c r="X2" s="198"/>
-      <c r="Y2" s="198"/>
-      <c r="Z2" s="198"/>
+      <c r="A2" s="183"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="183"/>
+      <c r="N2" s="183"/>
+      <c r="O2" s="183"/>
+      <c r="P2" s="183"/>
+      <c r="Q2" s="183"/>
+      <c r="R2" s="183"/>
+      <c r="S2" s="183"/>
+      <c r="T2" s="183"/>
+      <c r="U2" s="183"/>
+      <c r="V2" s="183"/>
+      <c r="W2" s="183"/>
+      <c r="X2" s="183"/>
+      <c r="Y2" s="183"/>
+      <c r="Z2" s="183"/>
     </row>
     <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="64" t="s">
@@ -2669,16 +2656,16 @@
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
       <c r="G3" s="65" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="163"/>
+        <v>102</v>
+      </c>
+      <c r="H3" s="162"/>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
-      <c r="N3" s="199"/>
-      <c r="O3" s="200"/>
+      <c r="N3" s="184"/>
+      <c r="O3" s="185"/>
       <c r="P3" s="67" t="s">
         <v>10</v>
       </c>
@@ -2695,49 +2682,49 @@
     </row>
     <row r="4" spans="1:26" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="138" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="138" t="s">
         <v>174</v>
       </c>
-      <c r="C4" s="138" t="s">
+      <c r="D4" s="171" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="172" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="184" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="185" t="s">
+      <c r="F4" s="172" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="185" t="s">
-        <v>177</v>
-      </c>
       <c r="G4" s="35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H4" s="143" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I4" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" s="143" t="s">
+        <v>163</v>
+      </c>
+      <c r="L4" s="143" t="s">
         <v>105</v>
       </c>
-      <c r="J4" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" s="143" t="s">
-        <v>164</v>
-      </c>
-      <c r="L4" s="143" t="s">
-        <v>106</v>
-      </c>
       <c r="M4" s="143" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N4" s="143" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O4" s="143" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P4" s="91" t="s">
         <v>55</v>
@@ -2755,50 +2742,50 @@
     </row>
     <row r="5" spans="1:26" s="27" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="186" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="186" t="s">
+      <c r="D5" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="186" t="s">
-        <v>178</v>
+      <c r="F5" s="173" t="s">
+        <v>177</v>
       </c>
       <c r="G5" s="139" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I5" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="J5" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="J5" s="37" t="s">
-        <v>163</v>
-      </c>
       <c r="K5" s="37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L5" s="139" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M5" s="37"/>
-      <c r="N5" s="191" t="s">
-        <v>136</v>
+      <c r="N5" s="178" t="s">
+        <v>135</v>
       </c>
       <c r="O5" s="37" t="s">
         <v>17</v>
       </c>
       <c r="P5" s="142" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q5" s="142"/>
       <c r="R5" s="38"/>
@@ -2815,19 +2802,19 @@
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="192"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="174"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="179"/>
       <c r="H6" s="40"/>
       <c r="I6" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K6" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L6" s="40"/>
       <c r="M6" s="40"/>
@@ -2870,7 +2857,7 @@
   <dimension ref="A1:BL6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2883,12 +2870,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="122" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="169" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
+      <c r="A1" s="192" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
       <c r="E1" s="12" t="s">
         <v>25</v>
       </c>
@@ -2902,7 +2889,7 @@
       <c r="E2" s="123"/>
       <c r="F2" s="123"/>
       <c r="G2" s="118" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H2" s="124"/>
       <c r="I2" s="124"/>
@@ -2972,71 +2959,71 @@
       <c r="G3" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="188">
+      <c r="H3" s="175">
         <v>1</v>
       </c>
-      <c r="I3" s="188">
+      <c r="I3" s="175">
         <v>2</v>
       </c>
-      <c r="J3" s="188">
+      <c r="J3" s="175">
         <v>3</v>
       </c>
-      <c r="K3" s="188" t="s">
+      <c r="K3" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="188"/>
-      <c r="M3" s="188"/>
-      <c r="N3" s="188"/>
-      <c r="O3" s="188"/>
-      <c r="P3" s="188"/>
-      <c r="Q3" s="188"/>
-      <c r="R3" s="188"/>
-      <c r="S3" s="188"/>
-      <c r="T3" s="188"/>
-      <c r="U3" s="188"/>
-      <c r="V3" s="188"/>
-      <c r="W3" s="188"/>
-      <c r="X3" s="188"/>
-      <c r="Y3" s="188"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="188"/>
-      <c r="AB3" s="188"/>
-      <c r="AC3" s="188"/>
-      <c r="AD3" s="188"/>
-      <c r="AE3" s="188"/>
-      <c r="AF3" s="188"/>
-      <c r="AG3" s="188"/>
-      <c r="AH3" s="188"/>
-      <c r="AI3" s="188"/>
-      <c r="AJ3" s="188"/>
-      <c r="AK3" s="188"/>
-      <c r="AL3" s="188"/>
-      <c r="AM3" s="188"/>
-      <c r="AN3" s="188"/>
-      <c r="AO3" s="188"/>
-      <c r="AP3" s="188"/>
-      <c r="AQ3" s="188"/>
-      <c r="AR3" s="188"/>
-      <c r="AS3" s="188"/>
-      <c r="AT3" s="189"/>
-      <c r="AU3" s="189"/>
-      <c r="AV3" s="189"/>
-      <c r="AW3" s="189"/>
-      <c r="AX3" s="189"/>
-      <c r="AY3" s="189"/>
-      <c r="AZ3" s="189"/>
-      <c r="BA3" s="189"/>
-      <c r="BB3" s="189"/>
-      <c r="BC3" s="189"/>
-      <c r="BD3" s="189"/>
-      <c r="BE3" s="189"/>
-      <c r="BF3" s="189"/>
-      <c r="BG3" s="189"/>
-      <c r="BH3" s="189"/>
-      <c r="BI3" s="189"/>
-      <c r="BJ3" s="189"/>
-      <c r="BK3" s="189"/>
-      <c r="BL3" s="189"/>
+      <c r="L3" s="175"/>
+      <c r="M3" s="175"/>
+      <c r="N3" s="175"/>
+      <c r="O3" s="175"/>
+      <c r="P3" s="175"/>
+      <c r="Q3" s="175"/>
+      <c r="R3" s="175"/>
+      <c r="S3" s="175"/>
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="Z3" s="175"/>
+      <c r="AA3" s="175"/>
+      <c r="AB3" s="175"/>
+      <c r="AC3" s="175"/>
+      <c r="AD3" s="175"/>
+      <c r="AE3" s="175"/>
+      <c r="AF3" s="175"/>
+      <c r="AG3" s="175"/>
+      <c r="AH3" s="175"/>
+      <c r="AI3" s="175"/>
+      <c r="AJ3" s="175"/>
+      <c r="AK3" s="175"/>
+      <c r="AL3" s="175"/>
+      <c r="AM3" s="175"/>
+      <c r="AN3" s="175"/>
+      <c r="AO3" s="175"/>
+      <c r="AP3" s="175"/>
+      <c r="AQ3" s="175"/>
+      <c r="AR3" s="175"/>
+      <c r="AS3" s="175"/>
+      <c r="AT3" s="176"/>
+      <c r="AU3" s="176"/>
+      <c r="AV3" s="176"/>
+      <c r="AW3" s="176"/>
+      <c r="AX3" s="176"/>
+      <c r="AY3" s="176"/>
+      <c r="AZ3" s="176"/>
+      <c r="BA3" s="176"/>
+      <c r="BB3" s="176"/>
+      <c r="BC3" s="176"/>
+      <c r="BD3" s="176"/>
+      <c r="BE3" s="176"/>
+      <c r="BF3" s="176"/>
+      <c r="BG3" s="176"/>
+      <c r="BH3" s="176"/>
+      <c r="BI3" s="176"/>
+      <c r="BJ3" s="176"/>
+      <c r="BK3" s="176"/>
+      <c r="BL3" s="176"/>
     </row>
     <row r="4" spans="1:64" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="130"/>
@@ -3108,16 +3095,16 @@
     </row>
     <row r="5" spans="1:64" ht="51" x14ac:dyDescent="0.15">
       <c r="A5" s="133" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" s="133" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="134" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E5" s="134" t="s">
         <v>55</v>
@@ -3131,19 +3118,19 @@
     </row>
     <row r="6" spans="1:64" s="136" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="135" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="135" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="135" t="s">
-        <v>102</v>
-      </c>
       <c r="C6" s="135" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="135" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="135" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" s="135" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="135" t="s">
-        <v>124</v>
       </c>
       <c r="F6" s="105" t="s">
         <v>58</v>
@@ -3185,7 +3172,7 @@
   <sheetData>
     <row r="1" spans="1:62" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="145" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="145"/>
       <c r="C1" s="147"/>
@@ -3195,11 +3182,11 @@
     </row>
     <row r="2" spans="1:62" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="95"/>
-      <c r="B2" s="161"/>
+      <c r="B2" s="160"/>
       <c r="C2" s="96"/>
       <c r="D2" s="96"/>
       <c r="E2" s="118" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -3267,71 +3254,71 @@
       <c r="E3" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="188">
+      <c r="F3" s="175">
         <v>1</v>
       </c>
-      <c r="G3" s="188">
+      <c r="G3" s="175">
         <v>2</v>
       </c>
-      <c r="H3" s="188">
+      <c r="H3" s="175">
         <v>3</v>
       </c>
-      <c r="I3" s="188" t="s">
+      <c r="I3" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="188"/>
-      <c r="K3" s="188"/>
-      <c r="L3" s="188"/>
-      <c r="M3" s="188"/>
-      <c r="N3" s="188"/>
-      <c r="O3" s="188"/>
-      <c r="P3" s="188"/>
-      <c r="Q3" s="188"/>
-      <c r="R3" s="188"/>
-      <c r="S3" s="188"/>
-      <c r="T3" s="188"/>
-      <c r="U3" s="188"/>
-      <c r="V3" s="188"/>
-      <c r="W3" s="188"/>
-      <c r="X3" s="188"/>
-      <c r="Y3" s="188"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="188"/>
-      <c r="AB3" s="188"/>
-      <c r="AC3" s="188"/>
-      <c r="AD3" s="188"/>
-      <c r="AE3" s="188"/>
-      <c r="AF3" s="188"/>
-      <c r="AG3" s="188"/>
-      <c r="AH3" s="188"/>
-      <c r="AI3" s="188"/>
-      <c r="AJ3" s="188"/>
-      <c r="AK3" s="188"/>
-      <c r="AL3" s="188"/>
-      <c r="AM3" s="188"/>
-      <c r="AN3" s="188"/>
-      <c r="AO3" s="188"/>
-      <c r="AP3" s="188"/>
-      <c r="AQ3" s="188"/>
-      <c r="AR3" s="189"/>
-      <c r="AS3" s="189"/>
-      <c r="AT3" s="189"/>
-      <c r="AU3" s="189"/>
-      <c r="AV3" s="189"/>
-      <c r="AW3" s="189"/>
-      <c r="AX3" s="189"/>
-      <c r="AY3" s="189"/>
-      <c r="AZ3" s="189"/>
-      <c r="BA3" s="189"/>
-      <c r="BB3" s="189"/>
-      <c r="BC3" s="189"/>
-      <c r="BD3" s="189"/>
-      <c r="BE3" s="189"/>
-      <c r="BF3" s="189"/>
-      <c r="BG3" s="189"/>
-      <c r="BH3" s="189"/>
-      <c r="BI3" s="189"/>
-      <c r="BJ3" s="189"/>
+      <c r="J3" s="175"/>
+      <c r="K3" s="175"/>
+      <c r="L3" s="175"/>
+      <c r="M3" s="175"/>
+      <c r="N3" s="175"/>
+      <c r="O3" s="175"/>
+      <c r="P3" s="175"/>
+      <c r="Q3" s="175"/>
+      <c r="R3" s="175"/>
+      <c r="S3" s="175"/>
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="Z3" s="175"/>
+      <c r="AA3" s="175"/>
+      <c r="AB3" s="175"/>
+      <c r="AC3" s="175"/>
+      <c r="AD3" s="175"/>
+      <c r="AE3" s="175"/>
+      <c r="AF3" s="175"/>
+      <c r="AG3" s="175"/>
+      <c r="AH3" s="175"/>
+      <c r="AI3" s="175"/>
+      <c r="AJ3" s="175"/>
+      <c r="AK3" s="175"/>
+      <c r="AL3" s="175"/>
+      <c r="AM3" s="175"/>
+      <c r="AN3" s="175"/>
+      <c r="AO3" s="175"/>
+      <c r="AP3" s="175"/>
+      <c r="AQ3" s="175"/>
+      <c r="AR3" s="176"/>
+      <c r="AS3" s="176"/>
+      <c r="AT3" s="176"/>
+      <c r="AU3" s="176"/>
+      <c r="AV3" s="176"/>
+      <c r="AW3" s="176"/>
+      <c r="AX3" s="176"/>
+      <c r="AY3" s="176"/>
+      <c r="AZ3" s="176"/>
+      <c r="BA3" s="176"/>
+      <c r="BB3" s="176"/>
+      <c r="BC3" s="176"/>
+      <c r="BD3" s="176"/>
+      <c r="BE3" s="176"/>
+      <c r="BF3" s="176"/>
+      <c r="BG3" s="176"/>
+      <c r="BH3" s="176"/>
+      <c r="BI3" s="176"/>
+      <c r="BJ3" s="176"/>
     </row>
     <row r="4" spans="1:62" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="99"/>
@@ -3401,10 +3388,10 @@
     </row>
     <row r="5" spans="1:62" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="134" t="s">
         <v>55</v>
@@ -3475,13 +3462,13 @@
     </row>
     <row r="6" spans="1:62" ht="78" x14ac:dyDescent="0.15">
       <c r="A6" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="162" t="s">
-        <v>188</v>
+        <v>107</v>
+      </c>
+      <c r="B6" s="161" t="s">
+        <v>187</v>
       </c>
       <c r="C6" s="135" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="105" t="s">
         <v>58</v>
@@ -3496,7 +3483,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
@@ -3565,7 +3552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAD3D8F-E56C-A042-B18B-973E8E62E26F}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView topLeftCell="Q1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3595,11 +3584,11 @@
   <sheetData>
     <row r="1" spans="1:26" s="22" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="114" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="114"/>
       <c r="C1" s="115"/>
-      <c r="E1" s="193" t="s">
+      <c r="E1" s="180" t="s">
         <v>25</v>
       </c>
       <c r="H1" s="23"/>
@@ -3623,8 +3612,8 @@
       <c r="Z1"/>
     </row>
     <row r="2" spans="1:26" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="166"/>
-      <c r="B2" s="180"/>
+      <c r="A2" s="165"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="62"/>
       <c r="D2" s="63"/>
       <c r="E2" s="62"/>
@@ -3651,22 +3640,22 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="1:26" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="172" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="173" t="s">
+      <c r="A3" s="193" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="194" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" s="80"/>
       <c r="F3" s="80"/>
       <c r="G3" s="80"/>
       <c r="H3" s="21"/>
       <c r="I3" s="85" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J3" s="85"/>
       <c r="K3" s="85"/>
@@ -3675,150 +3664,150 @@
       <c r="N3" s="85"/>
       <c r="O3" s="85"/>
       <c r="P3" s="21"/>
-      <c r="Q3" s="204" t="s">
+      <c r="Q3" s="195" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="204"/>
-      <c r="S3" s="204"/>
+      <c r="R3" s="195"/>
+      <c r="S3" s="195"/>
       <c r="T3" s="88"/>
       <c r="U3" s="88"/>
       <c r="V3" s="88"/>
       <c r="W3" s="21"/>
       <c r="X3" s="86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y3" s="86"/>
       <c r="Z3"/>
     </row>
     <row r="4" spans="1:26" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="157" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="164" t="s">
-        <v>179</v>
+        <v>138</v>
+      </c>
+      <c r="B4" s="163" t="s">
+        <v>178</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="57" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="156" t="s">
+        <v>211</v>
+      </c>
+      <c r="J4" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="K4" s="70" t="s">
+        <v>209</v>
+      </c>
+      <c r="L4" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="M4" s="70" t="s">
+        <v>222</v>
+      </c>
+      <c r="N4" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="O4" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="188" t="s">
+        <v>160</v>
+      </c>
+      <c r="R4" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="J4" s="70" t="s">
-        <v>224</v>
-      </c>
-      <c r="K4" s="70" t="s">
-        <v>212</v>
-      </c>
-      <c r="L4" s="70" t="s">
-        <v>159</v>
-      </c>
-      <c r="M4" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="N4" s="70" t="s">
+      <c r="S4" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="T4" s="188" t="s">
+        <v>213</v>
+      </c>
+      <c r="U4" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="V4" s="78" t="s">
         <v>151</v>
-      </c>
-      <c r="O4" s="70" t="s">
-        <v>160</v>
-      </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="203" t="s">
-        <v>161</v>
-      </c>
-      <c r="R4" s="78" t="s">
-        <v>217</v>
-      </c>
-      <c r="S4" s="78" t="s">
-        <v>150</v>
-      </c>
-      <c r="T4" s="203" t="s">
-        <v>216</v>
-      </c>
-      <c r="U4" s="78" t="s">
-        <v>218</v>
-      </c>
-      <c r="V4" s="78" t="s">
-        <v>152</v>
       </c>
       <c r="W4" s="15"/>
       <c r="X4" s="71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y4" s="71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Z4"/>
     </row>
     <row r="5" spans="1:26" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.15">
-      <c r="A5" s="165" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="165" t="s">
-        <v>186</v>
+      <c r="A5" s="164" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="164" t="s">
+        <v>185</v>
       </c>
       <c r="C5" s="148"/>
       <c r="D5" s="139" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="149" t="s">
-        <v>168</v>
-      </c>
-      <c r="F5" s="190" t="s">
-        <v>201</v>
+        <v>167</v>
+      </c>
+      <c r="F5" s="177" t="s">
+        <v>200</v>
       </c>
       <c r="G5" s="149" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H5" s="74"/>
-      <c r="I5" s="202" t="s">
-        <v>211</v>
-      </c>
-      <c r="J5" s="201"/>
-      <c r="K5" s="201" t="s">
-        <v>213</v>
-      </c>
-      <c r="L5" s="201" t="s">
-        <v>230</v>
-      </c>
-      <c r="M5" s="201" t="s">
-        <v>228</v>
-      </c>
-      <c r="N5" s="201" t="s">
+      <c r="I5" s="187" t="s">
+        <v>208</v>
+      </c>
+      <c r="J5" s="186"/>
+      <c r="K5" s="186" t="s">
+        <v>210</v>
+      </c>
+      <c r="L5" s="186" t="s">
         <v>227</v>
       </c>
-      <c r="O5" s="201" t="s">
-        <v>229</v>
+      <c r="M5" s="186" t="s">
+        <v>225</v>
+      </c>
+      <c r="N5" s="186" t="s">
+        <v>224</v>
+      </c>
+      <c r="O5" s="186" t="s">
+        <v>226</v>
       </c>
       <c r="P5" s="152"/>
       <c r="Q5" s="153" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R5" s="153"/>
       <c r="S5" s="153"/>
       <c r="T5" s="153" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="U5" s="153"/>
       <c r="V5" s="153" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="W5" s="148"/>
       <c r="X5" s="150" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y5" s="150" t="s">
         <v>115</v>
-      </c>
-      <c r="Y5" s="150" t="s">
-        <v>116</v>
       </c>
       <c r="Z5"/>
     </row>
@@ -3832,13 +3821,13 @@
       <c r="G6" s="48"/>
       <c r="H6" s="55"/>
       <c r="I6" s="47"/>
-      <c r="J6" s="205" t="s">
-        <v>221</v>
-      </c>
-      <c r="K6" s="205"/>
+      <c r="J6" s="189" t="s">
+        <v>218</v>
+      </c>
+      <c r="K6" s="189"/>
       <c r="L6" s="47"/>
-      <c r="M6" s="205" t="s">
-        <v>221</v>
+      <c r="M6" s="189" t="s">
+        <v>218</v>
       </c>
       <c r="N6" s="47"/>
       <c r="O6" s="47"/>
@@ -3849,14 +3838,14 @@
       <c r="T6" s="155"/>
       <c r="U6" s="155"/>
       <c r="V6" s="155" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W6" s="60"/>
       <c r="X6" s="154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y6" s="154" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z6"/>
     </row>
@@ -3939,7 +3928,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="22" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="114" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B1" s="114"/>
       <c r="C1" s="115"/>
@@ -3962,8 +3951,8 @@
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="170"/>
-      <c r="B2" s="171"/>
+      <c r="A2" s="196"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="62"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -3984,17 +3973,17 @@
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="172" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="173" t="s">
+      <c r="A3" s="193" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="194" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="174" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="174"/>
+      <c r="D3" s="198" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="198"/>
       <c r="F3" s="88"/>
       <c r="G3" s="88"/>
       <c r="H3" s="88"/>
@@ -4003,12 +3992,12 @@
       <c r="K3" s="88"/>
       <c r="L3" s="21"/>
       <c r="M3" s="86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N3" s="86"/>
       <c r="O3" s="21"/>
       <c r="P3" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
@@ -4017,42 +4006,42 @@
     </row>
     <row r="4" spans="1:20" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="157" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="164" t="s">
-        <v>207</v>
+        <v>138</v>
+      </c>
+      <c r="B4" s="163" t="s">
+        <v>204</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="78" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="78" t="s">
-        <v>144</v>
-      </c>
       <c r="G4" s="78" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H4" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="78" t="s">
         <v>166</v>
       </c>
-      <c r="I4" s="78" t="s">
-        <v>167</v>
-      </c>
       <c r="J4" s="78" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K4" s="78" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L4" s="15"/>
       <c r="M4" s="71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N4" s="71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O4" s="15"/>
       <c r="P4" s="72"/>
@@ -4063,42 +4052,42 @@
     </row>
     <row r="5" spans="1:20" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A5" s="151" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B5" s="151" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C5" s="148"/>
       <c r="D5" s="153" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="153" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="153" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="153" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="153" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="153" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" s="153" t="s">
-        <v>117</v>
-      </c>
-      <c r="G5" s="153" t="s">
-        <v>181</v>
-      </c>
-      <c r="H5" s="153" t="s">
+      <c r="I5" s="153" t="s">
+        <v>223</v>
+      </c>
+      <c r="J5" s="153" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="153" t="s">
-        <v>226</v>
-      </c>
-      <c r="J5" s="153" t="s">
-        <v>117</v>
-      </c>
       <c r="K5" s="153" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L5" s="148"/>
       <c r="M5" s="150" t="s">
+        <v>114</v>
+      </c>
+      <c r="N5" s="150" t="s">
         <v>115</v>
-      </c>
-      <c r="N5" s="150" t="s">
-        <v>116</v>
       </c>
       <c r="O5" s="148"/>
       <c r="P5" s="72"/>
@@ -4112,27 +4101,27 @@
       <c r="B6" s="109"/>
       <c r="C6" s="60"/>
       <c r="D6" s="155" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="155"/>
       <c r="F6" s="155" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="155"/>
       <c r="H6" s="155" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I6" s="155"/>
       <c r="J6" s="155" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K6" s="155"/>
       <c r="L6" s="60"/>
       <c r="M6" s="154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N6" s="154" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O6" s="60"/>
       <c r="P6" s="19"/>
@@ -4199,7 +4188,7 @@
   <sheetData>
     <row r="1" spans="1:64" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="145" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="146"/>
       <c r="C1" s="147"/>
@@ -4288,71 +4277,71 @@
       <c r="G3" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="188">
+      <c r="H3" s="175">
         <v>1</v>
       </c>
-      <c r="I3" s="188">
+      <c r="I3" s="175">
         <v>2</v>
       </c>
-      <c r="J3" s="188">
+      <c r="J3" s="175">
         <v>3</v>
       </c>
-      <c r="K3" s="188" t="s">
+      <c r="K3" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="188"/>
-      <c r="M3" s="188"/>
-      <c r="N3" s="188"/>
-      <c r="O3" s="188"/>
-      <c r="P3" s="188"/>
-      <c r="Q3" s="188"/>
-      <c r="R3" s="188"/>
-      <c r="S3" s="188"/>
-      <c r="T3" s="188"/>
-      <c r="U3" s="188"/>
-      <c r="V3" s="188"/>
-      <c r="W3" s="188"/>
-      <c r="X3" s="188"/>
-      <c r="Y3" s="188"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="188"/>
-      <c r="AB3" s="188"/>
-      <c r="AC3" s="188"/>
-      <c r="AD3" s="188"/>
-      <c r="AE3" s="188"/>
-      <c r="AF3" s="188"/>
-      <c r="AG3" s="188"/>
-      <c r="AH3" s="188"/>
-      <c r="AI3" s="188"/>
-      <c r="AJ3" s="188"/>
-      <c r="AK3" s="188"/>
-      <c r="AL3" s="188"/>
-      <c r="AM3" s="188"/>
-      <c r="AN3" s="188"/>
-      <c r="AO3" s="188"/>
-      <c r="AP3" s="188"/>
-      <c r="AQ3" s="188"/>
-      <c r="AR3" s="188"/>
-      <c r="AS3" s="188"/>
-      <c r="AT3" s="189"/>
-      <c r="AU3" s="189"/>
-      <c r="AV3" s="189"/>
-      <c r="AW3" s="189"/>
-      <c r="AX3" s="189"/>
-      <c r="AY3" s="189"/>
-      <c r="AZ3" s="189"/>
-      <c r="BA3" s="189"/>
-      <c r="BB3" s="189"/>
-      <c r="BC3" s="189"/>
-      <c r="BD3" s="189"/>
-      <c r="BE3" s="189"/>
-      <c r="BF3" s="189"/>
-      <c r="BG3" s="189"/>
-      <c r="BH3" s="189"/>
-      <c r="BI3" s="189"/>
-      <c r="BJ3" s="189"/>
-      <c r="BK3" s="189"/>
-      <c r="BL3" s="189"/>
+      <c r="L3" s="175"/>
+      <c r="M3" s="175"/>
+      <c r="N3" s="175"/>
+      <c r="O3" s="175"/>
+      <c r="P3" s="175"/>
+      <c r="Q3" s="175"/>
+      <c r="R3" s="175"/>
+      <c r="S3" s="175"/>
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="Z3" s="175"/>
+      <c r="AA3" s="175"/>
+      <c r="AB3" s="175"/>
+      <c r="AC3" s="175"/>
+      <c r="AD3" s="175"/>
+      <c r="AE3" s="175"/>
+      <c r="AF3" s="175"/>
+      <c r="AG3" s="175"/>
+      <c r="AH3" s="175"/>
+      <c r="AI3" s="175"/>
+      <c r="AJ3" s="175"/>
+      <c r="AK3" s="175"/>
+      <c r="AL3" s="175"/>
+      <c r="AM3" s="175"/>
+      <c r="AN3" s="175"/>
+      <c r="AO3" s="175"/>
+      <c r="AP3" s="175"/>
+      <c r="AQ3" s="175"/>
+      <c r="AR3" s="175"/>
+      <c r="AS3" s="175"/>
+      <c r="AT3" s="176"/>
+      <c r="AU3" s="176"/>
+      <c r="AV3" s="176"/>
+      <c r="AW3" s="176"/>
+      <c r="AX3" s="176"/>
+      <c r="AY3" s="176"/>
+      <c r="AZ3" s="176"/>
+      <c r="BA3" s="176"/>
+      <c r="BB3" s="176"/>
+      <c r="BC3" s="176"/>
+      <c r="BD3" s="176"/>
+      <c r="BE3" s="176"/>
+      <c r="BF3" s="176"/>
+      <c r="BG3" s="176"/>
+      <c r="BH3" s="176"/>
+      <c r="BI3" s="176"/>
+      <c r="BJ3" s="176"/>
+      <c r="BK3" s="176"/>
+      <c r="BL3" s="176"/>
     </row>
     <row r="4" spans="1:64" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="99"/>
@@ -4424,13 +4413,13 @@
     </row>
     <row r="5" spans="1:64" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="106" t="s">
         <v>128</v>
-      </c>
-      <c r="C5" s="106" t="s">
-        <v>129</v>
       </c>
       <c r="D5" s="106" t="s">
         <v>56</v>
@@ -4504,10 +4493,10 @@
     </row>
     <row r="6" spans="1:64" ht="52" x14ac:dyDescent="0.15">
       <c r="A6" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="144" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="105" t="s">
         <v>59</v>
@@ -4516,7 +4505,7 @@
         <v>29</v>
       </c>
       <c r="E6" s="105" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F6" s="105" t="s">
         <v>58</v>
@@ -4608,7 +4597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4641,7 +4632,7 @@
       <c r="C1" s="115"/>
       <c r="D1" s="115"/>
       <c r="E1" s="115"/>
-      <c r="F1" s="193" t="s">
+      <c r="F1" s="180" t="s">
         <v>25</v>
       </c>
       <c r="I1" s="29"/>
@@ -4657,8 +4648,8 @@
       <c r="S1" s="23"/>
     </row>
     <row r="2" spans="1:19" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="170"/>
-      <c r="B2" s="171"/>
+      <c r="A2" s="196"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="62"/>
       <c r="D2" s="63"/>
       <c r="E2" s="62"/>
@@ -4678,10 +4669,10 @@
       <c r="S2" s="23"/>
     </row>
     <row r="3" spans="1:19" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="172" t="s">
+      <c r="A3" s="193" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="173" t="s">
+      <c r="B3" s="194" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
@@ -4694,15 +4685,15 @@
       <c r="H3" s="80"/>
       <c r="I3" s="81"/>
       <c r="J3" s="21"/>
-      <c r="K3" s="178" t="s">
+      <c r="K3" s="168" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="179"/>
+      <c r="L3" s="169"/>
       <c r="M3" s="88"/>
       <c r="N3" s="88"/>
       <c r="O3" s="75"/>
       <c r="P3" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
@@ -4712,21 +4703,21 @@
       <c r="A4" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="164" t="s">
-        <v>189</v>
+      <c r="B4" s="163" t="s">
+        <v>188</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="57" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="57" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H4" s="58" t="s">
         <v>61</v>
@@ -4749,7 +4740,7 @@
       </c>
       <c r="O4" s="15"/>
       <c r="P4" s="72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q4" s="72"/>
       <c r="R4" s="158"/>
@@ -4757,10 +4748,10 @@
     </row>
     <row r="5" spans="1:19" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="117" t="s">
@@ -4770,10 +4761,10 @@
         <v>64</v>
       </c>
       <c r="F5" s="139" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H5" s="48" t="s">
         <v>16</v>
@@ -4786,7 +4777,7 @@
         <v>87</v>
       </c>
       <c r="L5" s="113" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M5" s="113" t="s">
         <v>85</v>
@@ -4795,8 +4786,8 @@
         <v>88</v>
       </c>
       <c r="O5" s="74"/>
-      <c r="P5" s="177" t="s">
-        <v>190</v>
+      <c r="P5" s="167" t="s">
+        <v>189</v>
       </c>
       <c r="Q5" s="19"/>
       <c r="R5" s="20"/>
@@ -4908,7 +4899,7 @@
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
-      <c r="F1" s="193" t="s">
+      <c r="F1" s="180" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="23"/>
@@ -4947,8 +4938,8 @@
       <c r="AN1" s="23"/>
     </row>
     <row r="2" spans="1:40" s="22" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="166"/>
-      <c r="B2" s="180"/>
+      <c r="A2" s="165"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -4989,17 +4980,17 @@
       <c r="AN2" s="23"/>
     </row>
     <row r="3" spans="1:40" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="175" t="s">
+      <c r="A3" s="199" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="176" t="s">
+      <c r="B3" s="200" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="174" t="s">
+      <c r="D3" s="198" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="174"/>
+      <c r="E3" s="198"/>
       <c r="F3" s="88"/>
       <c r="G3" s="88"/>
       <c r="H3" s="21"/>
@@ -5016,7 +5007,7 @@
       <c r="Q3" s="88"/>
       <c r="R3" s="21"/>
       <c r="S3" s="84" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="T3" s="85"/>
       <c r="U3" s="75"/>
@@ -5042,7 +5033,7 @@
       <c r="AI3" s="82"/>
       <c r="AJ3" s="75"/>
       <c r="AK3" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AL3" s="32"/>
       <c r="AM3" s="32"/>
@@ -5098,17 +5089,17 @@
       </c>
       <c r="R4" s="15"/>
       <c r="S4" s="70" t="s">
+        <v>196</v>
+      </c>
+      <c r="T4" s="70" t="s">
         <v>197</v>
-      </c>
-      <c r="T4" s="70" t="s">
-        <v>198</v>
       </c>
       <c r="U4" s="76"/>
       <c r="V4" s="71" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="W4" s="71" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X4" s="71" t="s">
         <v>81</v>
@@ -5121,26 +5112,26 @@
         <v>66</v>
       </c>
       <c r="AB4" s="69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC4" s="15"/>
       <c r="AD4" s="71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AE4" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF4" s="71" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG4" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="AF4" s="71" t="s">
-        <v>199</v>
-      </c>
-      <c r="AG4" s="71" t="s">
+      <c r="AH4" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="AH4" s="71" t="s">
+      <c r="AI4" s="71" t="s">
         <v>96</v>
-      </c>
-      <c r="AI4" s="71" t="s">
-        <v>97</v>
       </c>
       <c r="AJ4" s="15"/>
       <c r="AK4" s="72"/>
@@ -5150,10 +5141,10 @@
     </row>
     <row r="5" spans="1:40" s="68" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="74"/>
       <c r="D5" s="113" t="s">
@@ -5172,7 +5163,7 @@
       <c r="I5" s="79"/>
       <c r="J5" s="79"/>
       <c r="K5" s="113" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L5" s="79"/>
       <c r="M5" s="79"/>
@@ -5182,14 +5173,14 @@
       <c r="Q5" s="79"/>
       <c r="R5" s="74"/>
       <c r="S5" s="112" t="s">
+        <v>193</v>
+      </c>
+      <c r="T5" s="112" t="s">
         <v>194</v>
-      </c>
-      <c r="T5" s="112" t="s">
-        <v>195</v>
       </c>
       <c r="U5" s="77"/>
       <c r="V5" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="W5" s="49" t="s">
         <v>80</v>
@@ -5203,11 +5194,11 @@
         <v>67</v>
       </c>
       <c r="AB5" s="111" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC5" s="60"/>
       <c r="AD5" s="49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AE5" s="49"/>
       <c r="AF5" s="49" t="s">

</xml_diff>

<commit_message>
Updated template with more comments and added assets for Wiki
Todo: update validation for extra phase equilibria metadata
</commit_message>
<xml_diff>
--- a/templates/Experimental_Analyses_Template.xlsx
+++ b/templates/Experimental_Analyses_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmith/Downloads/Browser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmith/LEPR_traceDs/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF8FFE9-8865-1040-8BED-A2256DE08378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A4AEF6-5F24-FC4B-ADF0-34A833148DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31400" yWindow="-800" windowWidth="28820" windowHeight="18040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57140" yWindow="7860" windowWidth="28820" windowHeight="18040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Data Source" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="3 Bulk (Starting Materials)" sheetId="9" r:id="rId3"/>
     <sheet name="4 Bulk (Run Products)" sheetId="12" r:id="rId4"/>
     <sheet name="5 Primary Device Metadata" sheetId="10" r:id="rId5"/>
-    <sheet name="6 Device-specific Metadata " sheetId="13" r:id="rId6"/>
+    <sheet name="6 Device-specific Metadata" sheetId="13" r:id="rId6"/>
     <sheet name="7 Data" sheetId="4" r:id="rId7"/>
     <sheet name="8 Primary Method Metadata" sheetId="3" r:id="rId8"/>
     <sheet name="9 Method-specific Metadata" sheetId="2" r:id="rId9"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="242">
   <si>
     <t>Measured Parameter</t>
   </si>
@@ -443,9 +443,6 @@
   </si>
   <si>
     <t>must match a code in the DATA tab (or one of the BULK tabs) row 3</t>
-  </si>
-  <si>
-    <t>assign a number that links method to paramater(s); must match the DATA tab (or one of the BULK tabs) row 3</t>
   </si>
   <si>
     <t>EXPERIMENTAL PROCEDURE</t>
@@ -620,9 +617,6 @@
   </si>
   <si>
     <t>defaut is not reversed</t>
-  </si>
-  <si>
-    <t>optional descripion of a group of experiments (e.g. 'KLB-1 1GPa') or leave blank for all experiments in the same device</t>
   </si>
   <si>
     <t>Primary Device Metadata</t>
@@ -708,18 +702,9 @@
     <t>add ROR for laboratories not in current list, if available</t>
   </si>
   <si>
-    <t>optional descripion for  (e.g. 'volatiles', 'mineral', 'glass') or leave blank for all analyses in same batch</t>
-  </si>
-  <si>
     <t>experiment</t>
   </si>
   <si>
-    <t>assign a number that links experimental method to run(s); must match the EXPERIMENT tab column G</t>
-  </si>
-  <si>
-    <t>may match a run in the EXPERIMENT tab column A; or leave blank for all experiments with the same experimental method</t>
-  </si>
-  <si>
     <t>Device-specific Metadata</t>
   </si>
   <si>
@@ -750,9 +735,6 @@
     <t>e.g. oil pressure + friction correction, pressure marker</t>
   </si>
   <si>
-    <t>e.g. friction correction value</t>
-  </si>
-  <si>
     <t>units:</t>
   </si>
   <si>
@@ -783,13 +765,64 @@
     <t>e.g. WC, sintered diamond, diamond, moissanite</t>
   </si>
   <si>
-    <t>v3.0 last modified 11/26/2024</t>
-  </si>
-  <si>
     <t>Template developed by LEPR - IEDA2</t>
   </si>
   <si>
     <t>https://doi.org/10.60520/IEDA/113570</t>
+  </si>
+  <si>
+    <t>optional description for a species or group of species (e.g. 'volatiles', 'mineral', 'glass') or leave blank for all analyses in same batch</t>
+  </si>
+  <si>
+    <t>BOLD, CAPITAL headings indicate MANDATORY fields (temperature and pressure uncertainty may be entered here or on Sheet 6)</t>
+  </si>
+  <si>
+    <t>BOLD, CAPITAL headings indicate MANDATORY fields (temperature and pressure uncertainty may be entered here or on Sheet 5)</t>
+  </si>
+  <si>
+    <t>optional descripion of a group of experiments (e.g. 'KLB-1 1GPa') or leave blank for all experiments using the same device and setup</t>
+  </si>
+  <si>
+    <t>assign an alphanumeric code that links the experimental method for one or more runs; must match the EXPERIMENT tab column G</t>
+  </si>
+  <si>
+    <t>assign a number that links method to a group of paramaters; must match the DATA tab (or one of the BULK tabs) row 3</t>
+  </si>
+  <si>
+    <t>one row per unique device code:</t>
+  </si>
+  <si>
+    <t>one or more rows per device code:</t>
+  </si>
+  <si>
+    <t>may match a run in the EXPERIMENT tab column A; or leave blank for all experiments with the same device / experimental method</t>
+  </si>
+  <si>
+    <t>one row per unique method code:</t>
+  </si>
+  <si>
+    <t>one or more rows per method code:</t>
+  </si>
+  <si>
+    <t>one row per experiment:</t>
+  </si>
+  <si>
+    <t>e.g. friction correction value as bars or %</t>
+  </si>
+  <si>
+    <t>BOLD, CAPITAL headings indicate MANDATORY fields (some details may be given here or on Sheet 9)</t>
+  </si>
+  <si>
+    <t>BOLD, CAPITAL headings indicate MANDATORY fields (some details may be given here or on Sheet 8)</t>
+  </si>
+  <si>
+    <t>(if applicable)</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>v3.1 last modified 05/20/2025</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1111,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1229,8 +1262,32 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD5B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E4BC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8B7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1379,6 +1436,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1392,7 +1460,7 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1497,18 +1565,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1534,22 +1590,12 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1576,13 +1622,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1652,15 +1692,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1669,9 +1700,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1758,9 +1786,6 @@
     <xf numFmtId="0" fontId="20" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1783,7 +1808,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1798,10 +1822,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="40" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1848,16 +1868,135 @@
     <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="13" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1868,21 +2007,6 @@
     <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2296,7 +2420,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2308,101 +2432,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="218" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="201" t="s">
+      <c r="B1" s="219"/>
+      <c r="C1" s="171" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="159" t="s">
-        <v>229</v>
+      <c r="B2" s="144" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="202" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="203" t="s">
-        <v>230</v>
+      <c r="A3" s="172" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="173" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="53"/>
+      <c r="B4" s="49"/>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="46" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="45"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="46" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="45"/>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="46" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="45"/>
     </row>
     <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="46" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="45"/>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="46" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="45"/>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="46" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="45"/>
     </row>
     <row r="11" spans="1:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="46" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="45"/>
     </row>
-    <row r="13" spans="1:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="A13" s="89" t="s">
+    <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="A13" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="103" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="45"/>
@@ -2411,63 +2535,63 @@
       <c r="A14" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="50"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="45"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="50"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="45"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="50"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="45"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="50"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="45"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="50"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="50"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="50"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="45"/>
     </row>
-    <row r="23" spans="1:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="A23" s="89" t="s">
+    <row r="23" spans="1:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="A23" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="116" t="s">
+      <c r="B23" s="103" t="s">
         <v>90</v>
       </c>
       <c r="C23" s="45"/>
@@ -2476,60 +2600,60 @@
       <c r="A24" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="50"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="45"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="50"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="45"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="50"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="45"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="50"/>
+      <c r="B27" s="46"/>
       <c r="C27" s="45"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="50"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="45"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="50"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="45"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="50"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="45"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="50"/>
+      <c r="B31" s="46"/>
       <c r="C31" s="45"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="170" t="s">
+      <c r="A33" s="152" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2560,13 +2684,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="20" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" style="2" customWidth="1"/>
@@ -2578,132 +2700,132 @@
     <col min="12" max="12" width="20.83203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="18.1640625" style="2" customWidth="1"/>
     <col min="14" max="14" width="15.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" style="56" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" style="52" customWidth="1"/>
     <col min="16" max="16" width="21.83203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="15.33203125" style="2" customWidth="1"/>
     <col min="18" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="182" t="s">
+      <c r="B1" s="101"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="164" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="183"/>
-      <c r="I1" s="183"/>
-      <c r="J1" s="183"/>
-      <c r="K1" s="183"/>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
-      <c r="P1" s="183"/>
-      <c r="Q1" s="183"/>
-      <c r="R1" s="183"/>
-      <c r="S1" s="183"/>
-      <c r="T1" s="183"/>
-      <c r="U1" s="183"/>
-      <c r="V1" s="183"/>
-      <c r="W1" s="183"/>
-      <c r="X1" s="183"/>
-      <c r="Y1" s="183"/>
-      <c r="Z1" s="183"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="165"/>
+      <c r="K1" s="165"/>
+      <c r="L1" s="165"/>
+      <c r="M1" s="165"/>
+      <c r="N1" s="165"/>
+      <c r="O1" s="165"/>
+      <c r="P1" s="165"/>
+      <c r="Q1" s="165"/>
+      <c r="R1" s="165"/>
+      <c r="S1" s="165"/>
+      <c r="T1" s="165"/>
+      <c r="U1" s="165"/>
+      <c r="V1" s="165"/>
+      <c r="W1" s="165"/>
+      <c r="X1" s="165"/>
+      <c r="Y1" s="165"/>
+      <c r="Z1" s="165"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="183"/>
-      <c r="M2" s="183"/>
-      <c r="N2" s="183"/>
-      <c r="O2" s="183"/>
-      <c r="P2" s="183"/>
-      <c r="Q2" s="183"/>
-      <c r="R2" s="183"/>
-      <c r="S2" s="183"/>
-      <c r="T2" s="183"/>
-      <c r="U2" s="183"/>
-      <c r="V2" s="183"/>
-      <c r="W2" s="183"/>
-      <c r="X2" s="183"/>
-      <c r="Y2" s="183"/>
-      <c r="Z2" s="183"/>
+      <c r="A2" s="165"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="165"/>
+      <c r="U2" s="165"/>
+      <c r="V2" s="165"/>
+      <c r="W2" s="165"/>
+      <c r="X2" s="165"/>
+      <c r="Y2" s="165"/>
+      <c r="Z2" s="165"/>
     </row>
     <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="137"/>
+      <c r="B3" s="123"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="176" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="162"/>
+      <c r="H3" s="146"/>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
-      <c r="N3" s="184"/>
-      <c r="O3" s="185"/>
-      <c r="P3" s="67" t="s">
+      <c r="N3" s="166"/>
+      <c r="O3" s="167"/>
+      <c r="P3" s="59" t="s">
         <v>10</v>
       </c>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
       <c r="S3" s="33"/>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="80"/>
     </row>
     <row r="4" spans="1:26" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="124" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="124" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="138" t="s">
+      <c r="D4" s="153" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="154" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="171" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="172" t="s">
+      <c r="F4" s="154" t="s">
         <v>175</v>
-      </c>
-      <c r="F4" s="172" t="s">
-        <v>176</v>
       </c>
       <c r="G4" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="143" t="s">
-        <v>183</v>
+      <c r="H4" s="129" t="s">
+        <v>182</v>
       </c>
       <c r="I4" s="35" t="s">
         <v>104</v>
@@ -2711,34 +2833,34 @@
       <c r="J4" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="K4" s="143" t="s">
-        <v>163</v>
-      </c>
-      <c r="L4" s="143" t="s">
+      <c r="K4" s="129" t="s">
+        <v>162</v>
+      </c>
+      <c r="L4" s="129" t="s">
         <v>105</v>
       </c>
-      <c r="M4" s="143" t="s">
-        <v>182</v>
-      </c>
-      <c r="N4" s="143" t="s">
-        <v>134</v>
-      </c>
-      <c r="O4" s="143" t="s">
-        <v>136</v>
-      </c>
-      <c r="P4" s="91" t="s">
+      <c r="M4" s="129" t="s">
+        <v>181</v>
+      </c>
+      <c r="N4" s="129" t="s">
+        <v>133</v>
+      </c>
+      <c r="O4" s="129" t="s">
+        <v>135</v>
+      </c>
+      <c r="P4" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="92"/>
-      <c r="U4" s="92"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92"/>
-      <c r="X4" s="92"/>
-      <c r="Y4" s="92"/>
-      <c r="Z4" s="92"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="82"/>
+      <c r="X4" s="82"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="82"/>
     </row>
     <row r="5" spans="1:26" s="27" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="36" t="s">
@@ -2747,65 +2869,67 @@
       <c r="B5" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="140" t="s">
+      <c r="C5" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="173" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="173" t="s">
+      <c r="D5" s="155" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="173" t="s">
-        <v>177</v>
-      </c>
-      <c r="G5" s="139" t="s">
+      <c r="F5" s="155" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="125" t="s">
         <v>125</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I5" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="J5" s="37" t="s">
         <v>161</v>
-      </c>
-      <c r="J5" s="37" t="s">
-        <v>162</v>
       </c>
       <c r="K5" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="L5" s="139" t="s">
+      <c r="L5" s="125" t="s">
         <v>124</v>
       </c>
       <c r="M5" s="37"/>
-      <c r="N5" s="178" t="s">
-        <v>135</v>
+      <c r="N5" s="160" t="s">
+        <v>134</v>
       </c>
       <c r="O5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="142" t="s">
+      <c r="P5" s="128" t="s">
         <v>123</v>
       </c>
-      <c r="Q5" s="142"/>
+      <c r="Q5" s="128"/>
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
-      <c r="T5" s="93"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="93"/>
-      <c r="Y5" s="93"/>
-      <c r="Z5" s="93"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A6" s="39"/>
+      <c r="A6" s="203" t="s">
+        <v>235</v>
+      </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
-      <c r="D6" s="174"/>
-      <c r="E6" s="174"/>
-      <c r="F6" s="174"/>
-      <c r="G6" s="179"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="161"/>
       <c r="H6" s="40"/>
       <c r="I6" s="40" t="s">
         <v>113</v>
@@ -2818,19 +2942,19 @@
       </c>
       <c r="L6" s="40"/>
       <c r="M6" s="40"/>
-      <c r="N6" s="149"/>
+      <c r="N6" s="135"/>
       <c r="O6" s="37"/>
       <c r="P6" s="41"/>
       <c r="Q6" s="41"/>
       <c r="R6" s="41"/>
       <c r="S6" s="41"/>
-      <c r="T6" s="94"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="94"/>
-      <c r="W6" s="94"/>
-      <c r="X6" s="94"/>
-      <c r="Y6" s="94"/>
-      <c r="Z6" s="94"/>
+      <c r="T6" s="84"/>
+      <c r="U6" s="84"/>
+      <c r="V6" s="84"/>
+      <c r="W6" s="84"/>
+      <c r="X6" s="84"/>
+      <c r="Y6" s="84"/>
+      <c r="Z6" s="84"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -2856,293 +2980,288 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB839336-BA14-2045-A8D0-963F349663C6}">
   <dimension ref="A1:BL6"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="128" customWidth="1"/>
-    <col min="2" max="5" width="15.6640625" style="128" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="128" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" style="128" customWidth="1"/>
-    <col min="8" max="16384" width="10.6640625" style="128"/>
+    <col min="1" max="1" width="17.33203125" style="114" customWidth="1"/>
+    <col min="2" max="5" width="15.6640625" style="114" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="114" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="114" customWidth="1"/>
+    <col min="8" max="16384" width="10.6640625" style="114"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="122" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="192" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
+    <row r="1" spans="1:64" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A1" s="217" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
       <c r="E1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="121"/>
+      <c r="G1" s="107"/>
     </row>
     <row r="2" spans="1:64" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="95"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="118" t="s">
-        <v>155</v>
-      </c>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="126"/>
-      <c r="AA2" s="126"/>
-      <c r="AB2" s="126"/>
-      <c r="AC2" s="126"/>
-      <c r="AD2" s="126"/>
-      <c r="AE2" s="126"/>
-      <c r="AF2" s="126"/>
-      <c r="AG2" s="126"/>
-      <c r="AH2" s="126"/>
-      <c r="AI2" s="126"/>
-      <c r="AJ2" s="126"/>
-      <c r="AK2" s="126"/>
-      <c r="AL2" s="126"/>
-      <c r="AM2" s="126"/>
-      <c r="AN2" s="126"/>
-      <c r="AO2" s="126"/>
-      <c r="AP2" s="126"/>
-      <c r="AQ2" s="126"/>
-      <c r="AR2" s="126"/>
-      <c r="AS2" s="126"/>
-      <c r="AT2" s="126"/>
-      <c r="AU2" s="127"/>
-      <c r="AV2" s="127"/>
-      <c r="AW2" s="127"/>
-      <c r="AX2" s="127"/>
-      <c r="AY2" s="127"/>
-      <c r="AZ2" s="127"/>
-      <c r="BA2" s="127"/>
-      <c r="BB2" s="127"/>
-      <c r="BC2" s="127"/>
-      <c r="BD2" s="127"/>
-      <c r="BE2" s="127"/>
-      <c r="BF2" s="127"/>
-      <c r="BG2" s="127"/>
-      <c r="BH2" s="127"/>
-      <c r="BI2" s="127"/>
-      <c r="BJ2" s="127"/>
-      <c r="BK2" s="127"/>
-      <c r="BL2" s="127"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="104" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="112"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="112"/>
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="112"/>
+      <c r="AF2" s="112"/>
+      <c r="AG2" s="112"/>
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="112"/>
+      <c r="AJ2" s="112"/>
+      <c r="AK2" s="112"/>
+      <c r="AL2" s="112"/>
+      <c r="AM2" s="112"/>
+      <c r="AN2" s="112"/>
+      <c r="AO2" s="112"/>
+      <c r="AP2" s="112"/>
+      <c r="AQ2" s="112"/>
+      <c r="AR2" s="112"/>
+      <c r="AS2" s="112"/>
+      <c r="AT2" s="112"/>
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="113"/>
+      <c r="AY2" s="113"/>
+      <c r="AZ2" s="113"/>
+      <c r="BA2" s="113"/>
+      <c r="BB2" s="113"/>
+      <c r="BC2" s="113"/>
+      <c r="BD2" s="113"/>
+      <c r="BE2" s="113"/>
+      <c r="BF2" s="113"/>
+      <c r="BG2" s="113"/>
+      <c r="BH2" s="113"/>
+      <c r="BI2" s="113"/>
+      <c r="BJ2" s="113"/>
+      <c r="BK2" s="113"/>
+      <c r="BL2" s="113"/>
     </row>
     <row r="3" spans="1:64" ht="34" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="129"/>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="119" t="s">
+      <c r="A3" s="115"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="175">
+      <c r="H3" s="157">
         <v>1</v>
       </c>
-      <c r="I3" s="175">
+      <c r="I3" s="157">
         <v>2</v>
       </c>
-      <c r="J3" s="175">
+      <c r="J3" s="157">
         <v>3</v>
       </c>
-      <c r="K3" s="175" t="s">
+      <c r="K3" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="175"/>
-      <c r="AA3" s="175"/>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="175"/>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="175"/>
-      <c r="AG3" s="175"/>
-      <c r="AH3" s="175"/>
-      <c r="AI3" s="175"/>
-      <c r="AJ3" s="175"/>
-      <c r="AK3" s="175"/>
-      <c r="AL3" s="175"/>
-      <c r="AM3" s="175"/>
-      <c r="AN3" s="175"/>
-      <c r="AO3" s="175"/>
-      <c r="AP3" s="175"/>
-      <c r="AQ3" s="175"/>
-      <c r="AR3" s="175"/>
-      <c r="AS3" s="175"/>
-      <c r="AT3" s="176"/>
-      <c r="AU3" s="176"/>
-      <c r="AV3" s="176"/>
-      <c r="AW3" s="176"/>
-      <c r="AX3" s="176"/>
-      <c r="AY3" s="176"/>
-      <c r="AZ3" s="176"/>
-      <c r="BA3" s="176"/>
-      <c r="BB3" s="176"/>
-      <c r="BC3" s="176"/>
-      <c r="BD3" s="176"/>
-      <c r="BE3" s="176"/>
-      <c r="BF3" s="176"/>
-      <c r="BG3" s="176"/>
-      <c r="BH3" s="176"/>
-      <c r="BI3" s="176"/>
-      <c r="BJ3" s="176"/>
-      <c r="BK3" s="176"/>
-      <c r="BL3" s="176"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="157"/>
+      <c r="N3" s="157"/>
+      <c r="O3" s="157"/>
+      <c r="P3" s="157"/>
+      <c r="Q3" s="157"/>
+      <c r="R3" s="157"/>
+      <c r="S3" s="157"/>
+      <c r="T3" s="157"/>
+      <c r="U3" s="157"/>
+      <c r="V3" s="157"/>
+      <c r="W3" s="157"/>
+      <c r="X3" s="157"/>
+      <c r="Y3" s="157"/>
+      <c r="Z3" s="157"/>
+      <c r="AA3" s="157"/>
+      <c r="AB3" s="157"/>
+      <c r="AC3" s="157"/>
+      <c r="AD3" s="157"/>
+      <c r="AE3" s="157"/>
+      <c r="AF3" s="157"/>
+      <c r="AG3" s="157"/>
+      <c r="AH3" s="157"/>
+      <c r="AI3" s="157"/>
+      <c r="AJ3" s="157"/>
+      <c r="AK3" s="157"/>
+      <c r="AL3" s="157"/>
+      <c r="AM3" s="157"/>
+      <c r="AN3" s="157"/>
+      <c r="AO3" s="157"/>
+      <c r="AP3" s="157"/>
+      <c r="AQ3" s="157"/>
+      <c r="AR3" s="157"/>
+      <c r="AS3" s="157"/>
+      <c r="AT3" s="158"/>
+      <c r="AU3" s="158"/>
+      <c r="AV3" s="158"/>
+      <c r="AW3" s="158"/>
+      <c r="AX3" s="158"/>
+      <c r="AY3" s="158"/>
+      <c r="AZ3" s="158"/>
+      <c r="BA3" s="158"/>
+      <c r="BB3" s="158"/>
+      <c r="BC3" s="158"/>
+      <c r="BD3" s="158"/>
+      <c r="BE3" s="158"/>
+      <c r="BF3" s="158"/>
+      <c r="BG3" s="158"/>
+      <c r="BH3" s="158"/>
+      <c r="BI3" s="158"/>
+      <c r="BJ3" s="158"/>
+      <c r="BK3" s="158"/>
+      <c r="BL3" s="158"/>
     </row>
     <row r="4" spans="1:64" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="130"/>
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="141" t="s">
+      <c r="A4" s="116"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="131"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="131"/>
-      <c r="O4" s="131"/>
-      <c r="P4" s="131"/>
-      <c r="Q4" s="131"/>
-      <c r="R4" s="131"/>
-      <c r="S4" s="131"/>
-      <c r="T4" s="131"/>
-      <c r="U4" s="131"/>
-      <c r="V4" s="131"/>
-      <c r="W4" s="131"/>
-      <c r="X4" s="131"/>
-      <c r="Y4" s="131"/>
-      <c r="Z4" s="131"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="131"/>
-      <c r="AD4" s="131"/>
-      <c r="AE4" s="131"/>
-      <c r="AF4" s="131"/>
-      <c r="AG4" s="131"/>
-      <c r="AH4" s="131"/>
-      <c r="AI4" s="131"/>
-      <c r="AJ4" s="131"/>
-      <c r="AK4" s="131"/>
-      <c r="AL4" s="131"/>
-      <c r="AM4" s="131"/>
-      <c r="AN4" s="131"/>
-      <c r="AO4" s="131"/>
-      <c r="AP4" s="131"/>
-      <c r="AQ4" s="131"/>
-      <c r="AR4" s="131"/>
-      <c r="AS4" s="131"/>
-      <c r="AT4" s="132"/>
-      <c r="AU4" s="132"/>
-      <c r="AV4" s="132"/>
-      <c r="AW4" s="132"/>
-      <c r="AX4" s="132"/>
-      <c r="AY4" s="132"/>
-      <c r="AZ4" s="132"/>
-      <c r="BA4" s="132"/>
-      <c r="BB4" s="132"/>
-      <c r="BC4" s="132"/>
-      <c r="BD4" s="132"/>
-      <c r="BE4" s="132"/>
-      <c r="BF4" s="132"/>
-      <c r="BG4" s="132"/>
-      <c r="BH4" s="132"/>
-      <c r="BI4" s="132"/>
-      <c r="BJ4" s="132"/>
-      <c r="BK4" s="132"/>
-      <c r="BL4" s="132"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
+      <c r="N4" s="117"/>
+      <c r="O4" s="117"/>
+      <c r="P4" s="117"/>
+      <c r="Q4" s="117"/>
+      <c r="R4" s="117"/>
+      <c r="S4" s="117"/>
+      <c r="T4" s="117"/>
+      <c r="U4" s="117"/>
+      <c r="V4" s="117"/>
+      <c r="W4" s="117"/>
+      <c r="X4" s="117"/>
+      <c r="Y4" s="117"/>
+      <c r="Z4" s="117"/>
+      <c r="AA4" s="117"/>
+      <c r="AB4" s="117"/>
+      <c r="AC4" s="117"/>
+      <c r="AD4" s="117"/>
+      <c r="AE4" s="117"/>
+      <c r="AF4" s="117"/>
+      <c r="AG4" s="117"/>
+      <c r="AH4" s="117"/>
+      <c r="AI4" s="117"/>
+      <c r="AJ4" s="117"/>
+      <c r="AK4" s="117"/>
+      <c r="AL4" s="117"/>
+      <c r="AM4" s="117"/>
+      <c r="AN4" s="117"/>
+      <c r="AO4" s="117"/>
+      <c r="AP4" s="117"/>
+      <c r="AQ4" s="117"/>
+      <c r="AR4" s="117"/>
+      <c r="AS4" s="117"/>
+      <c r="AT4" s="118"/>
+      <c r="AU4" s="118"/>
+      <c r="AV4" s="118"/>
+      <c r="AW4" s="118"/>
+      <c r="AX4" s="118"/>
+      <c r="AY4" s="118"/>
+      <c r="AZ4" s="118"/>
+      <c r="BA4" s="118"/>
+      <c r="BB4" s="118"/>
+      <c r="BC4" s="118"/>
+      <c r="BD4" s="118"/>
+      <c r="BE4" s="118"/>
+      <c r="BF4" s="118"/>
+      <c r="BG4" s="118"/>
+      <c r="BH4" s="118"/>
+      <c r="BI4" s="118"/>
+      <c r="BJ4" s="118"/>
+      <c r="BK4" s="118"/>
+      <c r="BL4" s="118"/>
     </row>
     <row r="5" spans="1:64" ht="51" x14ac:dyDescent="0.15">
-      <c r="A5" s="133" t="s">
+      <c r="A5" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="120" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="134" t="s">
-        <v>146</v>
-      </c>
-      <c r="E5" s="134" t="s">
+      <c r="D5" s="120" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="96" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="43" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="136" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="135" t="s">
+    <row r="6" spans="1:64" s="122" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="135" t="s">
+      <c r="C6" s="121" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="135" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" s="135" t="s">
+      <c r="D6" s="121" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="121" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="105" t="s">
+      <c r="F6" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="104" t="s">
+      <c r="G6" s="94" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{24A1B706-C29C-A948-8CA6-65265C2A8653}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{9909E65C-DA4E-BC4F-8793-933E9F38603D}"/>
@@ -3171,22 +3290,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="147"/>
+      <c r="A1" s="131" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="133"/>
       <c r="D1" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:62" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="95"/>
-      <c r="B2" s="160"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="118" t="s">
-        <v>156</v>
+      <c r="A2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="104" t="s">
+        <v>155</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -3247,159 +3366,159 @@
       <c r="BJ2" s="1"/>
     </row>
     <row r="3" spans="1:62" ht="34" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="97"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="119" t="s">
+      <c r="A3" s="87"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="175">
+      <c r="F3" s="157">
         <v>1</v>
       </c>
-      <c r="G3" s="175">
+      <c r="G3" s="157">
         <v>2</v>
       </c>
-      <c r="H3" s="175">
+      <c r="H3" s="157">
         <v>3</v>
       </c>
-      <c r="I3" s="175" t="s">
+      <c r="I3" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="175"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="175"/>
-      <c r="AA3" s="175"/>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="175"/>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="175"/>
-      <c r="AG3" s="175"/>
-      <c r="AH3" s="175"/>
-      <c r="AI3" s="175"/>
-      <c r="AJ3" s="175"/>
-      <c r="AK3" s="175"/>
-      <c r="AL3" s="175"/>
-      <c r="AM3" s="175"/>
-      <c r="AN3" s="175"/>
-      <c r="AO3" s="175"/>
-      <c r="AP3" s="175"/>
-      <c r="AQ3" s="175"/>
-      <c r="AR3" s="176"/>
-      <c r="AS3" s="176"/>
-      <c r="AT3" s="176"/>
-      <c r="AU3" s="176"/>
-      <c r="AV3" s="176"/>
-      <c r="AW3" s="176"/>
-      <c r="AX3" s="176"/>
-      <c r="AY3" s="176"/>
-      <c r="AZ3" s="176"/>
-      <c r="BA3" s="176"/>
-      <c r="BB3" s="176"/>
-      <c r="BC3" s="176"/>
-      <c r="BD3" s="176"/>
-      <c r="BE3" s="176"/>
-      <c r="BF3" s="176"/>
-      <c r="BG3" s="176"/>
-      <c r="BH3" s="176"/>
-      <c r="BI3" s="176"/>
-      <c r="BJ3" s="176"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="157"/>
+      <c r="N3" s="157"/>
+      <c r="O3" s="157"/>
+      <c r="P3" s="157"/>
+      <c r="Q3" s="157"/>
+      <c r="R3" s="157"/>
+      <c r="S3" s="157"/>
+      <c r="T3" s="157"/>
+      <c r="U3" s="157"/>
+      <c r="V3" s="157"/>
+      <c r="W3" s="157"/>
+      <c r="X3" s="157"/>
+      <c r="Y3" s="157"/>
+      <c r="Z3" s="157"/>
+      <c r="AA3" s="157"/>
+      <c r="AB3" s="157"/>
+      <c r="AC3" s="157"/>
+      <c r="AD3" s="157"/>
+      <c r="AE3" s="157"/>
+      <c r="AF3" s="157"/>
+      <c r="AG3" s="157"/>
+      <c r="AH3" s="157"/>
+      <c r="AI3" s="157"/>
+      <c r="AJ3" s="157"/>
+      <c r="AK3" s="157"/>
+      <c r="AL3" s="157"/>
+      <c r="AM3" s="157"/>
+      <c r="AN3" s="157"/>
+      <c r="AO3" s="157"/>
+      <c r="AP3" s="157"/>
+      <c r="AQ3" s="157"/>
+      <c r="AR3" s="158"/>
+      <c r="AS3" s="158"/>
+      <c r="AT3" s="158"/>
+      <c r="AU3" s="158"/>
+      <c r="AV3" s="158"/>
+      <c r="AW3" s="158"/>
+      <c r="AX3" s="158"/>
+      <c r="AY3" s="158"/>
+      <c r="AZ3" s="158"/>
+      <c r="BA3" s="158"/>
+      <c r="BB3" s="158"/>
+      <c r="BC3" s="158"/>
+      <c r="BD3" s="158"/>
+      <c r="BE3" s="158"/>
+      <c r="BF3" s="158"/>
+      <c r="BG3" s="158"/>
+      <c r="BH3" s="158"/>
+      <c r="BI3" s="158"/>
+      <c r="BJ3" s="158"/>
     </row>
     <row r="4" spans="1:62" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="99"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="141" t="s">
+      <c r="A4" s="89"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="102"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="102"/>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="102"/>
-      <c r="AB4" s="102"/>
-      <c r="AC4" s="102"/>
-      <c r="AD4" s="102"/>
-      <c r="AE4" s="102"/>
-      <c r="AF4" s="102"/>
-      <c r="AG4" s="102"/>
-      <c r="AH4" s="102"/>
-      <c r="AI4" s="102"/>
-      <c r="AJ4" s="102"/>
-      <c r="AK4" s="102"/>
-      <c r="AL4" s="102"/>
-      <c r="AM4" s="102"/>
-      <c r="AN4" s="102"/>
-      <c r="AO4" s="102"/>
-      <c r="AP4" s="102"/>
-      <c r="AQ4" s="102"/>
-      <c r="AR4" s="103"/>
-      <c r="AS4" s="103"/>
-      <c r="AT4" s="103"/>
-      <c r="AU4" s="103"/>
-      <c r="AV4" s="103"/>
-      <c r="AW4" s="103"/>
-      <c r="AX4" s="103"/>
-      <c r="AY4" s="103"/>
-      <c r="AZ4" s="103"/>
-      <c r="BA4" s="103"/>
-      <c r="BB4" s="103"/>
-      <c r="BC4" s="103"/>
-      <c r="BD4" s="103"/>
-      <c r="BE4" s="103"/>
-      <c r="BF4" s="103"/>
-      <c r="BG4" s="103"/>
-      <c r="BH4" s="103"/>
-      <c r="BI4" s="103"/>
-      <c r="BJ4" s="103"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92"/>
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="92"/>
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="92"/>
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="92"/>
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="93"/>
+      <c r="AS4" s="93"/>
+      <c r="AT4" s="93"/>
+      <c r="AU4" s="93"/>
+      <c r="AV4" s="93"/>
+      <c r="AW4" s="93"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="93"/>
+      <c r="AZ4" s="93"/>
+      <c r="BA4" s="93"/>
+      <c r="BB4" s="93"/>
+      <c r="BC4" s="93"/>
+      <c r="BD4" s="93"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="93"/>
+      <c r="BG4" s="93"/>
+      <c r="BH4" s="93"/>
+      <c r="BI4" s="93"/>
+      <c r="BJ4" s="93"/>
     </row>
     <row r="5" spans="1:62" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="106" t="s">
+      <c r="D5" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="106" t="s">
+      <c r="E5" s="96" t="s">
         <v>53</v>
       </c>
       <c r="F5" s="2"/>
@@ -3464,16 +3583,16 @@
       <c r="A6" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="161" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" s="135" t="s">
+      <c r="B6" s="145" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="121" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="95" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="11"/>
@@ -3552,44 +3671,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAD3D8F-E56C-A042-B18B-973E8E62E26F}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="0.83203125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="0.83203125" style="51" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="7" width="21.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="1" style="55" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1" style="51" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.83203125" style="2" customWidth="1"/>
     <col min="12" max="13" width="21" style="2" customWidth="1"/>
     <col min="14" max="14" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="1" style="55" customWidth="1"/>
+    <col min="16" max="16" width="1" style="51" customWidth="1"/>
     <col min="17" max="17" width="17.5" customWidth="1"/>
     <col min="18" max="18" width="16.5" customWidth="1"/>
     <col min="19" max="19" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="15.83203125" customWidth="1"/>
-    <col min="23" max="23" width="0.83203125" style="55" customWidth="1"/>
-    <col min="24" max="24" width="19" style="2" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" customWidth="1"/>
+    <col min="21" max="21" width="18" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" customWidth="1"/>
+    <col min="23" max="23" width="0.83203125" style="51" customWidth="1"/>
+    <col min="24" max="24" width="20.1640625" style="2" customWidth="1"/>
     <col min="25" max="25" width="19.83203125" style="2" customWidth="1"/>
     <col min="27" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="22" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="114" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="115"/>
-      <c r="E1" s="180" t="s">
-        <v>25</v>
+      <c r="A1" s="101" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="102"/>
+      <c r="E1" s="162" t="s">
+        <v>225</v>
       </c>
       <c r="H1" s="23"/>
       <c r="I1" s="25"/>
@@ -3612,11 +3731,11 @@
       <c r="Z1"/>
     </row>
     <row r="2" spans="1:26" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="165"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="62"/>
+      <c r="A2" s="149"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="162"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -3640,226 +3759,228 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="1:26" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="193" t="s">
+      <c r="A3" s="220" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="221" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="75" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="222" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="222"/>
+      <c r="S3" s="222"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y3" s="76"/>
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:26" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="142" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="194" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="80" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="85" t="s">
+      <c r="B4" s="147" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="141" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" s="62" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="62" t="s">
+        <v>204</v>
+      </c>
+      <c r="L4" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="N4" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="O4" s="62" t="s">
+        <v>158</v>
+      </c>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="170" t="s">
+        <v>159</v>
+      </c>
+      <c r="R4" s="69" t="s">
+        <v>209</v>
+      </c>
+      <c r="S4" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="195" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="195"/>
-      <c r="S3" s="195"/>
-      <c r="T3" s="88"/>
-      <c r="U3" s="88"/>
-      <c r="V3" s="88"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="86" t="s">
+      <c r="T4" s="170" t="s">
+        <v>208</v>
+      </c>
+      <c r="U4" s="69" t="s">
+        <v>210</v>
+      </c>
+      <c r="V4" s="69" t="s">
+        <v>150</v>
+      </c>
+      <c r="W4" s="15"/>
+      <c r="X4" s="174" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y4" s="174" t="s">
         <v>140</v>
       </c>
-      <c r="Y3" s="86"/>
-      <c r="Z3"/>
-    </row>
-    <row r="4" spans="1:26" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="157" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="163" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="58" t="s">
-        <v>172</v>
-      </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="156" t="s">
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:26" s="28" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+      <c r="A5" s="148" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="148" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="134"/>
+      <c r="D5" s="125" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="135" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="159" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="169" t="s">
+        <v>203</v>
+      </c>
+      <c r="J5" s="168"/>
+      <c r="K5" s="168" t="s">
+        <v>205</v>
+      </c>
+      <c r="L5" s="168" t="s">
+        <v>221</v>
+      </c>
+      <c r="M5" s="168" t="s">
+        <v>219</v>
+      </c>
+      <c r="N5" s="168" t="s">
+        <v>218</v>
+      </c>
+      <c r="O5" s="168" t="s">
+        <v>220</v>
+      </c>
+      <c r="P5" s="137"/>
+      <c r="Q5" s="138" t="s">
+        <v>207</v>
+      </c>
+      <c r="R5" s="138"/>
+      <c r="S5" s="138"/>
+      <c r="T5" s="138" t="s">
         <v>211</v>
       </c>
-      <c r="J4" s="70" t="s">
-        <v>221</v>
-      </c>
-      <c r="K4" s="70" t="s">
-        <v>209</v>
-      </c>
-      <c r="L4" s="70" t="s">
-        <v>158</v>
-      </c>
-      <c r="M4" s="70" t="s">
-        <v>222</v>
-      </c>
-      <c r="N4" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="O4" s="70" t="s">
-        <v>159</v>
-      </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="188" t="s">
-        <v>160</v>
-      </c>
-      <c r="R4" s="78" t="s">
-        <v>214</v>
-      </c>
-      <c r="S4" s="78" t="s">
-        <v>149</v>
-      </c>
-      <c r="T4" s="188" t="s">
-        <v>213</v>
-      </c>
-      <c r="U4" s="78" t="s">
-        <v>215</v>
-      </c>
-      <c r="V4" s="78" t="s">
-        <v>151</v>
-      </c>
-      <c r="W4" s="15"/>
-      <c r="X4" s="71" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y4" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z4"/>
-    </row>
-    <row r="5" spans="1:26" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.15">
-      <c r="A5" s="164" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" s="164" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="139" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="149" t="s">
-        <v>167</v>
-      </c>
-      <c r="F5" s="177" t="s">
-        <v>200</v>
-      </c>
-      <c r="G5" s="149" t="s">
-        <v>202</v>
-      </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="187" t="s">
-        <v>208</v>
-      </c>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186" t="s">
-        <v>210</v>
-      </c>
-      <c r="L5" s="186" t="s">
-        <v>227</v>
-      </c>
-      <c r="M5" s="186" t="s">
-        <v>225</v>
-      </c>
-      <c r="N5" s="186" t="s">
-        <v>224</v>
-      </c>
-      <c r="O5" s="186" t="s">
-        <v>226</v>
-      </c>
-      <c r="P5" s="152"/>
-      <c r="Q5" s="153" t="s">
+      <c r="U5" s="138"/>
+      <c r="V5" s="138" t="s">
+        <v>236</v>
+      </c>
+      <c r="W5" s="134"/>
+      <c r="X5" s="136" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y5" s="136" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z5"/>
+    </row>
+    <row r="6" spans="1:26" s="183" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+      <c r="A6" s="184" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="185"/>
+      <c r="C6" s="177"/>
+      <c r="D6" s="178"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="207"/>
+      <c r="I6" s="204"/>
+      <c r="J6" s="181" t="s">
         <v>212</v>
       </c>
-      <c r="R5" s="153"/>
-      <c r="S5" s="153"/>
-      <c r="T5" s="153" t="s">
-        <v>216</v>
-      </c>
-      <c r="U5" s="153"/>
-      <c r="V5" s="153" t="s">
-        <v>217</v>
-      </c>
-      <c r="W5" s="148"/>
-      <c r="X5" s="150" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y5" s="150" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z5"/>
-    </row>
-    <row r="6" spans="1:26" s="28" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A6" s="109"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="189" t="s">
-        <v>218</v>
-      </c>
-      <c r="K6" s="189"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="189" t="s">
-        <v>218</v>
-      </c>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="155"/>
-      <c r="R6" s="155"/>
-      <c r="S6" s="155"/>
-      <c r="T6" s="155"/>
-      <c r="U6" s="155"/>
-      <c r="V6" s="155" t="s">
+      <c r="K6" s="181"/>
+      <c r="L6" s="180"/>
+      <c r="M6" s="181" t="s">
+        <v>212</v>
+      </c>
+      <c r="N6" s="180"/>
+      <c r="O6" s="180"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="140"/>
+      <c r="R6" s="140"/>
+      <c r="S6" s="140"/>
+      <c r="T6" s="140"/>
+      <c r="U6" s="140"/>
+      <c r="V6" s="140" t="s">
+        <v>212</v>
+      </c>
+      <c r="W6" s="177"/>
+      <c r="X6" s="139" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y6" s="139" t="s">
         <v>112</v>
       </c>
-      <c r="W6" s="60"/>
-      <c r="X6" s="154" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y6" s="154" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z6"/>
-    </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.15">
-      <c r="A7" s="110">
+      <c r="Z6" s="182"/>
+    </row>
+    <row r="7" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="100">
         <v>1</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="55"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="55"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -3867,24 +3988,24 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="74"/>
-      <c r="W7" s="55"/>
+      <c r="P7" s="51"/>
+      <c r="W7" s="51"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A8" s="110">
+      <c r="A8" s="100">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A9" s="110">
+      <c r="A9" s="100">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="100" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3914,26 +4035,28 @@
   <cols>
     <col min="1" max="1" width="21.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="0.83203125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="0.83203125" style="51" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="15.83203125" customWidth="1"/>
-    <col min="12" max="12" width="0.83203125" style="55" customWidth="1"/>
-    <col min="13" max="13" width="19" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="0.83203125" style="55" customWidth="1"/>
+    <col min="12" max="12" width="0.83203125" style="51" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="0.83203125" style="51" customWidth="1"/>
     <col min="16" max="18" width="10.6640625" style="2"/>
     <col min="21" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="22" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="114" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="115"/>
+      <c r="A1" s="101" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="E1" s="162" t="s">
+        <v>226</v>
+      </c>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
@@ -3951,9 +4074,9 @@
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="196"/>
-      <c r="B2" s="197"/>
-      <c r="C2" s="62"/>
+      <c r="A2" s="223"/>
+      <c r="B2" s="224"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
@@ -3973,31 +4096,31 @@
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="193" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="194" t="s">
+      <c r="A3" s="220" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="221" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="225" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="225"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="198"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="86" t="s">
-        <v>140</v>
-      </c>
-      <c r="N3" s="86"/>
+      <c r="N3" s="76"/>
       <c r="O3" s="21"/>
       <c r="P3" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
@@ -4005,125 +4128,127 @@
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="157" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="163" t="s">
-        <v>204</v>
+      <c r="A4" s="142" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="147" t="s">
+        <v>201</v>
       </c>
       <c r="C4" s="15"/>
-      <c r="D4" s="78" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="78" t="s">
+      <c r="D4" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="69" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="78" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="78" t="s">
-        <v>219</v>
-      </c>
-      <c r="H4" s="78" t="s">
+      <c r="G4" s="69" t="s">
+        <v>213</v>
+      </c>
+      <c r="H4" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="I4" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="J4" s="78" t="s">
-        <v>164</v>
-      </c>
-      <c r="K4" s="78" t="s">
-        <v>220</v>
+      <c r="J4" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="K4" s="69" t="s">
+        <v>214</v>
       </c>
       <c r="L4" s="15"/>
-      <c r="M4" s="71" t="s">
+      <c r="M4" s="174" t="s">
         <v>117</v>
       </c>
-      <c r="N4" s="71" t="s">
-        <v>141</v>
+      <c r="N4" s="174" t="s">
+        <v>140</v>
       </c>
       <c r="O4" s="15"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
       <c r="T4"/>
     </row>
-    <row r="5" spans="1:20" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.2">
-      <c r="A5" s="151" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" s="151" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="153" t="s">
+    <row r="5" spans="1:20" s="28" customFormat="1" ht="78" x14ac:dyDescent="0.2">
+      <c r="A5" s="148" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="134"/>
+      <c r="D5" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="153" t="s">
-        <v>181</v>
-      </c>
-      <c r="F5" s="153" t="s">
+      <c r="E5" s="138" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="138" t="s">
         <v>116</v>
       </c>
-      <c r="G5" s="153" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="153" t="s">
+      <c r="G5" s="138" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" s="138" t="s">
         <v>115</v>
       </c>
-      <c r="I5" s="153" t="s">
-        <v>223</v>
-      </c>
-      <c r="J5" s="153" t="s">
+      <c r="I5" s="138" t="s">
+        <v>217</v>
+      </c>
+      <c r="J5" s="138" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="153" t="s">
-        <v>179</v>
-      </c>
-      <c r="L5" s="148"/>
-      <c r="M5" s="150" t="s">
+      <c r="K5" s="138" t="s">
+        <v>178</v>
+      </c>
+      <c r="L5" s="134"/>
+      <c r="M5" s="136" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="150" t="s">
+      <c r="N5" s="136" t="s">
         <v>115</v>
       </c>
-      <c r="O5" s="148"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
       <c r="T5"/>
     </row>
     <row r="6" spans="1:20" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="109"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="155" t="s">
+      <c r="A6" s="184" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="185"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155" t="s">
+      <c r="E6" s="140"/>
+      <c r="F6" s="140" t="s">
         <v>110</v>
       </c>
-      <c r="G6" s="155"/>
-      <c r="H6" s="155" t="s">
+      <c r="G6" s="140"/>
+      <c r="H6" s="140" t="s">
         <v>112</v>
       </c>
-      <c r="I6" s="155"/>
-      <c r="J6" s="155" t="s">
+      <c r="I6" s="140"/>
+      <c r="J6" s="140" t="s">
         <v>110</v>
       </c>
-      <c r="K6" s="155"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="154" t="s">
+      <c r="K6" s="140"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="139" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="154" t="s">
+      <c r="N6" s="139" t="s">
         <v>112</v>
       </c>
-      <c r="O6" s="60"/>
+      <c r="O6" s="56"/>
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
       <c r="R6" s="20"/>
@@ -4131,30 +4256,30 @@
       <c r="T6"/>
     </row>
     <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="110">
+      <c r="A7" s="100">
         <v>1</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="C7" s="51"/>
+      <c r="L7" s="51"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="55"/>
+      <c r="O7" s="51"/>
       <c r="S7"/>
       <c r="T7"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8" s="110">
+      <c r="A8" s="100">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9" s="110">
+      <c r="A9" s="100">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="100" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4187,26 +4312,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="131" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="147"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="133"/>
       <c r="D1" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="101"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="2" spans="1:64" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="95"/>
-      <c r="B2" s="96"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="86"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="118" t="s">
+      <c r="G2" s="104" t="s">
         <v>50</v>
       </c>
       <c r="H2" s="5"/>
@@ -4268,148 +4393,148 @@
       <c r="BL2" s="1"/>
     </row>
     <row r="3" spans="1:64" ht="34" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="97"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="119" t="s">
+      <c r="A3" s="87"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="175">
+      <c r="H3" s="157">
         <v>1</v>
       </c>
-      <c r="I3" s="175">
+      <c r="I3" s="157">
         <v>2</v>
       </c>
-      <c r="J3" s="175">
+      <c r="J3" s="157">
         <v>3</v>
       </c>
-      <c r="K3" s="175" t="s">
+      <c r="K3" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="175"/>
-      <c r="AA3" s="175"/>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="175"/>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="175"/>
-      <c r="AG3" s="175"/>
-      <c r="AH3" s="175"/>
-      <c r="AI3" s="175"/>
-      <c r="AJ3" s="175"/>
-      <c r="AK3" s="175"/>
-      <c r="AL3" s="175"/>
-      <c r="AM3" s="175"/>
-      <c r="AN3" s="175"/>
-      <c r="AO3" s="175"/>
-      <c r="AP3" s="175"/>
-      <c r="AQ3" s="175"/>
-      <c r="AR3" s="175"/>
-      <c r="AS3" s="175"/>
-      <c r="AT3" s="176"/>
-      <c r="AU3" s="176"/>
-      <c r="AV3" s="176"/>
-      <c r="AW3" s="176"/>
-      <c r="AX3" s="176"/>
-      <c r="AY3" s="176"/>
-      <c r="AZ3" s="176"/>
-      <c r="BA3" s="176"/>
-      <c r="BB3" s="176"/>
-      <c r="BC3" s="176"/>
-      <c r="BD3" s="176"/>
-      <c r="BE3" s="176"/>
-      <c r="BF3" s="176"/>
-      <c r="BG3" s="176"/>
-      <c r="BH3" s="176"/>
-      <c r="BI3" s="176"/>
-      <c r="BJ3" s="176"/>
-      <c r="BK3" s="176"/>
-      <c r="BL3" s="176"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="157"/>
+      <c r="N3" s="157"/>
+      <c r="O3" s="157"/>
+      <c r="P3" s="157"/>
+      <c r="Q3" s="157"/>
+      <c r="R3" s="157"/>
+      <c r="S3" s="157"/>
+      <c r="T3" s="157"/>
+      <c r="U3" s="157"/>
+      <c r="V3" s="157"/>
+      <c r="W3" s="157"/>
+      <c r="X3" s="157"/>
+      <c r="Y3" s="157"/>
+      <c r="Z3" s="157"/>
+      <c r="AA3" s="157"/>
+      <c r="AB3" s="157"/>
+      <c r="AC3" s="157"/>
+      <c r="AD3" s="157"/>
+      <c r="AE3" s="157"/>
+      <c r="AF3" s="157"/>
+      <c r="AG3" s="157"/>
+      <c r="AH3" s="157"/>
+      <c r="AI3" s="157"/>
+      <c r="AJ3" s="157"/>
+      <c r="AK3" s="157"/>
+      <c r="AL3" s="157"/>
+      <c r="AM3" s="157"/>
+      <c r="AN3" s="157"/>
+      <c r="AO3" s="157"/>
+      <c r="AP3" s="157"/>
+      <c r="AQ3" s="157"/>
+      <c r="AR3" s="157"/>
+      <c r="AS3" s="157"/>
+      <c r="AT3" s="158"/>
+      <c r="AU3" s="158"/>
+      <c r="AV3" s="158"/>
+      <c r="AW3" s="158"/>
+      <c r="AX3" s="158"/>
+      <c r="AY3" s="158"/>
+      <c r="AZ3" s="158"/>
+      <c r="BA3" s="158"/>
+      <c r="BB3" s="158"/>
+      <c r="BC3" s="158"/>
+      <c r="BD3" s="158"/>
+      <c r="BE3" s="158"/>
+      <c r="BF3" s="158"/>
+      <c r="BG3" s="158"/>
+      <c r="BH3" s="158"/>
+      <c r="BI3" s="158"/>
+      <c r="BJ3" s="158"/>
+      <c r="BK3" s="158"/>
+      <c r="BL3" s="158"/>
     </row>
     <row r="4" spans="1:64" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="99"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="119" t="s">
+      <c r="A4" s="89"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="102"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="102"/>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="102"/>
-      <c r="AB4" s="102"/>
-      <c r="AC4" s="102"/>
-      <c r="AD4" s="102"/>
-      <c r="AE4" s="102"/>
-      <c r="AF4" s="102"/>
-      <c r="AG4" s="102"/>
-      <c r="AH4" s="102"/>
-      <c r="AI4" s="102"/>
-      <c r="AJ4" s="102"/>
-      <c r="AK4" s="102"/>
-      <c r="AL4" s="102"/>
-      <c r="AM4" s="102"/>
-      <c r="AN4" s="102"/>
-      <c r="AO4" s="102"/>
-      <c r="AP4" s="102"/>
-      <c r="AQ4" s="102"/>
-      <c r="AR4" s="102"/>
-      <c r="AS4" s="102"/>
-      <c r="AT4" s="103"/>
-      <c r="AU4" s="103"/>
-      <c r="AV4" s="103"/>
-      <c r="AW4" s="103"/>
-      <c r="AX4" s="103"/>
-      <c r="AY4" s="103"/>
-      <c r="AZ4" s="103"/>
-      <c r="BA4" s="103"/>
-      <c r="BB4" s="103"/>
-      <c r="BC4" s="103"/>
-      <c r="BD4" s="103"/>
-      <c r="BE4" s="103"/>
-      <c r="BF4" s="103"/>
-      <c r="BG4" s="103"/>
-      <c r="BH4" s="103"/>
-      <c r="BI4" s="103"/>
-      <c r="BJ4" s="103"/>
-      <c r="BK4" s="103"/>
-      <c r="BL4" s="103"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92"/>
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
+      <c r="T4" s="92"/>
+      <c r="U4" s="92"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="92"/>
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="92"/>
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="92"/>
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="92"/>
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="93"/>
+      <c r="AU4" s="93"/>
+      <c r="AV4" s="93"/>
+      <c r="AW4" s="93"/>
+      <c r="AX4" s="93"/>
+      <c r="AY4" s="93"/>
+      <c r="AZ4" s="93"/>
+      <c r="BA4" s="93"/>
+      <c r="BB4" s="93"/>
+      <c r="BC4" s="93"/>
+      <c r="BD4" s="93"/>
+      <c r="BE4" s="93"/>
+      <c r="BF4" s="93"/>
+      <c r="BG4" s="93"/>
+      <c r="BH4" s="93"/>
+      <c r="BI4" s="93"/>
+      <c r="BJ4" s="93"/>
+      <c r="BK4" s="93"/>
+      <c r="BL4" s="93"/>
     </row>
     <row r="5" spans="1:64" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="42" t="s">
@@ -4418,19 +4543,19 @@
       <c r="B5" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="106" t="s">
+      <c r="D5" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="106" t="s">
+      <c r="E5" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="216" t="s">
         <v>53</v>
       </c>
       <c r="H5" s="2"/>
@@ -4495,22 +4620,22 @@
       <c r="A6" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="130" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="105" t="s">
+      <c r="F6" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="104" t="s">
+      <c r="G6" s="94" t="s">
         <v>54</v>
       </c>
       <c r="H6" s="11"/>
@@ -4595,45 +4720,43 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:XFD10"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="0.83203125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="0.83203125" style="51" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="19.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="56" customWidth="1"/>
-    <col min="10" max="10" width="1" style="55" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="52" customWidth="1"/>
+    <col min="10" max="10" width="1" style="51" customWidth="1"/>
     <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.83203125" customWidth="1"/>
-    <col min="15" max="15" width="1" style="55" customWidth="1"/>
+    <col min="15" max="15" width="1" style="51" customWidth="1"/>
     <col min="16" max="16" width="21.6640625" style="2" customWidth="1"/>
     <col min="17" max="17" width="16.33203125" style="2" customWidth="1"/>
     <col min="18" max="19" width="10.6640625" style="2"/>
     <col min="27" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="22" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:19 16384:16384" s="22" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="101" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="180" t="s">
-        <v>25</v>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="162" t="s">
+        <v>237</v>
       </c>
       <c r="I1" s="29"/>
       <c r="J1" s="23"/>
@@ -4647,12 +4770,12 @@
       <c r="R1" s="23"/>
       <c r="S1" s="23"/>
     </row>
-    <row r="2" spans="1:19" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="196"/>
-      <c r="B2" s="197"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="62"/>
+    <row r="2" spans="1:19 16384:16384" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="223"/>
+      <c r="B2" s="224"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="26"/>
@@ -4668,162 +4791,177 @@
       <c r="R2" s="23"/>
       <c r="S2" s="23"/>
     </row>
-    <row r="3" spans="1:19" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="193" t="s">
+    <row r="3" spans="1:19 16384:16384" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="220" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="194" t="s">
+      <c r="B3" s="221" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="21"/>
-      <c r="K3" s="168" t="s">
+      <c r="K3" s="186" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="169"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="75"/>
+      <c r="L3" s="151"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="67"/>
       <c r="P3" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
       <c r="S3" s="32"/>
     </row>
-    <row r="4" spans="1:19" s="16" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="157" t="s">
+    <row r="4" spans="1:19 16384:16384" s="16" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="163" t="s">
-        <v>188</v>
+      <c r="B4" s="147" t="s">
+        <v>186</v>
       </c>
       <c r="C4" s="15"/>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="58" t="s">
-        <v>172</v>
-      </c>
-      <c r="H4" s="58" t="s">
+      <c r="G4" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="55" t="s">
         <v>62</v>
       </c>
       <c r="J4" s="15"/>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="78" t="s">
+      <c r="N4" s="69" t="s">
         <v>78</v>
       </c>
       <c r="O4" s="15"/>
-      <c r="P4" s="72" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="158"/>
-      <c r="S4" s="158"/>
-    </row>
-    <row r="5" spans="1:19" s="28" customFormat="1" ht="65" x14ac:dyDescent="0.2">
-      <c r="A5" s="109" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="109" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="117" t="s">
+      <c r="P4" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="143"/>
+      <c r="S4" s="143"/>
+    </row>
+    <row r="5" spans="1:19 16384:16384" s="28" customFormat="1" ht="78" x14ac:dyDescent="0.2">
+      <c r="A5" s="148" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="148" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" s="134"/>
+      <c r="D5" s="187" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="135" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="139" t="s">
-        <v>200</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>199</v>
-      </c>
-      <c r="H5" s="48" t="s">
+      <c r="F5" s="125" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="135" t="s">
+        <v>197</v>
+      </c>
+      <c r="H5" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="61" t="s">
+      <c r="I5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="113" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="138" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="113" t="s">
-        <v>171</v>
-      </c>
-      <c r="M5" s="113" t="s">
+      <c r="L5" s="138" t="s">
+        <v>170</v>
+      </c>
+      <c r="M5" s="138" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="113" t="s">
+      <c r="N5" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="O5" s="74"/>
-      <c r="P5" s="167" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-    </row>
-    <row r="6" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="110">
+      <c r="O5" s="15"/>
+      <c r="P5" s="188" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+    </row>
+    <row r="6" spans="1:19 16384:16384" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="201" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="191"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="193"/>
+      <c r="E6" s="194"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="194"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="198" t="s">
+        <v>239</v>
+      </c>
+      <c r="L6" s="198"/>
+      <c r="M6" s="198"/>
+      <c r="N6" s="198"/>
+      <c r="O6" s="177"/>
+      <c r="P6" s="199"/>
+      <c r="Q6" s="199"/>
+      <c r="R6" s="200"/>
+      <c r="S6" s="200"/>
+      <c r="XFD6" s="189"/>
+    </row>
+    <row r="7" spans="1:19 16384:16384" x14ac:dyDescent="0.15">
+      <c r="A7" s="100">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="55"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6" s="55"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A7" s="110">
+    </row>
+    <row r="8" spans="1:19 16384:16384" x14ac:dyDescent="0.15">
+      <c r="A8" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A8" s="110">
+      <c r="B8" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19 16384:16384" x14ac:dyDescent="0.15">
+      <c r="A9" s="100">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A9" s="110" t="s">
+    <row r="10" spans="1:19 16384:16384" x14ac:dyDescent="0.15">
+      <c r="A10" s="100" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4853,54 +4991,54 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AN9"/>
+  <dimension ref="A1:AN15"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="1" style="55" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="1" style="51" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1" style="55" customWidth="1"/>
+    <col min="8" max="8" width="1" style="51" customWidth="1"/>
     <col min="9" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" customWidth="1"/>
     <col min="14" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="0.83203125" style="55" customWidth="1"/>
+    <col min="18" max="18" width="0.83203125" style="51" customWidth="1"/>
     <col min="19" max="19" width="19.1640625" style="2" customWidth="1"/>
     <col min="20" max="20" width="16" style="2" customWidth="1"/>
-    <col min="21" max="21" width="1" style="55" customWidth="1"/>
+    <col min="21" max="21" width="1" style="51" customWidth="1"/>
     <col min="22" max="22" width="18.1640625" style="2" customWidth="1"/>
     <col min="23" max="23" width="17.83203125" style="2" customWidth="1"/>
     <col min="24" max="24" width="15" style="2" customWidth="1"/>
-    <col min="25" max="25" width="1" style="55" customWidth="1"/>
+    <col min="25" max="25" width="1" style="51" customWidth="1"/>
     <col min="26" max="26" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9" style="2" customWidth="1"/>
     <col min="28" max="28" width="16.6640625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="0.83203125" style="55" customWidth="1"/>
+    <col min="29" max="29" width="1.1640625" style="51" customWidth="1"/>
     <col min="30" max="30" width="19" style="2" customWidth="1"/>
     <col min="31" max="31" width="19.6640625" style="2" customWidth="1"/>
     <col min="32" max="32" width="15.5" style="2" customWidth="1"/>
     <col min="33" max="34" width="17.6640625" style="2" customWidth="1"/>
     <col min="35" max="35" width="13.6640625" style="2" customWidth="1"/>
-    <col min="36" max="36" width="1" style="55" customWidth="1"/>
+    <col min="36" max="36" width="0.83203125" style="51" customWidth="1"/>
     <col min="37" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="22" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="115"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
-      <c r="F1" s="180" t="s">
-        <v>25</v>
+      <c r="F1" s="162" t="s">
+        <v>238</v>
       </c>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
@@ -4913,7 +5051,7 @@
       <c r="O1" s="23"/>
       <c r="P1" s="23"/>
       <c r="Q1" s="23"/>
-      <c r="R1" s="115"/>
+      <c r="R1" s="102"/>
       <c r="S1" s="25"/>
       <c r="T1" s="23"/>
       <c r="U1" s="23"/>
@@ -4921,9 +5059,9 @@
       <c r="W1" s="23"/>
       <c r="X1" s="23"/>
       <c r="Y1" s="23"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="115"/>
-      <c r="AB1" s="115"/>
+      <c r="Z1" s="102"/>
+      <c r="AA1" s="102"/>
+      <c r="AB1" s="102"/>
       <c r="AC1" s="23"/>
       <c r="AD1" s="23"/>
       <c r="AE1" s="23"/>
@@ -4938,8 +5076,8 @@
       <c r="AN1" s="23"/>
     </row>
     <row r="2" spans="1:40" s="22" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="165"/>
-      <c r="B2" s="166"/>
+      <c r="A2" s="149"/>
+      <c r="B2" s="150"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -4955,7 +5093,7 @@
       <c r="O2" s="23"/>
       <c r="P2" s="23"/>
       <c r="Q2" s="23"/>
-      <c r="R2" s="62"/>
+      <c r="R2" s="57"/>
       <c r="S2" s="24"/>
       <c r="T2" s="23"/>
       <c r="U2" s="23"/>
@@ -4963,7 +5101,7 @@
       <c r="W2" s="23"/>
       <c r="X2" s="23"/>
       <c r="Y2" s="23"/>
-      <c r="Z2" s="63"/>
+      <c r="Z2" s="58"/>
       <c r="AA2" s="23"/>
       <c r="AB2" s="23"/>
       <c r="AC2" s="23"/>
@@ -4980,268 +5118,314 @@
       <c r="AN2" s="23"/>
     </row>
     <row r="3" spans="1:40" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="199" t="s">
+      <c r="A3" s="220" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="221" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
-      <c r="D3" s="198" t="s">
+      <c r="D3" s="222" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="198"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
       <c r="H3" s="21"/>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
       <c r="R3" s="21"/>
-      <c r="S3" s="84" t="s">
-        <v>192</v>
-      </c>
-      <c r="T3" s="85"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="86" t="s">
+      <c r="S3" s="74" t="s">
+        <v>190</v>
+      </c>
+      <c r="T3" s="75"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
+      <c r="W3" s="77"/>
+      <c r="X3" s="77"/>
       <c r="Y3" s="21"/>
-      <c r="Z3" s="83" t="s">
+      <c r="Z3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="80"/>
-      <c r="AB3" s="80"/>
+      <c r="AA3" s="70"/>
+      <c r="AB3" s="70"/>
       <c r="AC3" s="21"/>
-      <c r="AD3" s="86" t="s">
+      <c r="AD3" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="82"/>
-      <c r="AF3" s="82"/>
-      <c r="AG3" s="82"/>
-      <c r="AH3" s="82"/>
-      <c r="AI3" s="82"/>
-      <c r="AJ3" s="75"/>
+      <c r="AE3" s="72"/>
+      <c r="AF3" s="72"/>
+      <c r="AG3" s="72"/>
+      <c r="AH3" s="72"/>
+      <c r="AI3" s="72"/>
+      <c r="AJ3" s="67"/>
       <c r="AK3" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AL3" s="32"/>
       <c r="AM3" s="32"/>
       <c r="AN3" s="32"/>
     </row>
-    <row r="4" spans="1:40" s="68" customFormat="1" ht="51" x14ac:dyDescent="0.15">
-      <c r="A4" s="157" t="s">
+    <row r="4" spans="1:40" s="60" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+      <c r="A4" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="142" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="15"/>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="78" t="s">
+      <c r="G4" s="69" t="s">
         <v>78</v>
       </c>
       <c r="H4" s="15"/>
-      <c r="I4" s="78" t="s">
+      <c r="I4" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="N4" s="78" t="s">
+      <c r="N4" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="O4" s="78" t="s">
+      <c r="O4" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="P4" s="78" t="s">
+      <c r="P4" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="Q4" s="78" t="s">
+      <c r="Q4" s="69" t="s">
         <v>76</v>
       </c>
       <c r="R4" s="15"/>
-      <c r="S4" s="70" t="s">
+      <c r="S4" s="62" t="s">
+        <v>194</v>
+      </c>
+      <c r="T4" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="U4" s="68"/>
+      <c r="V4" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="W4" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="X4" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA4" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE4" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF4" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="T4" s="70" t="s">
-        <v>197</v>
-      </c>
-      <c r="U4" s="76"/>
-      <c r="V4" s="71" t="s">
-        <v>195</v>
-      </c>
-      <c r="W4" s="71" t="s">
-        <v>168</v>
-      </c>
-      <c r="X4" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA4" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB4" s="69" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE4" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF4" s="71" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG4" s="71" t="s">
+      <c r="AG4" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="AH4" s="71" t="s">
+      <c r="AH4" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="AI4" s="71" t="s">
+      <c r="AI4" s="63" t="s">
         <v>96</v>
       </c>
       <c r="AJ4" s="15"/>
-      <c r="AK4" s="72"/>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="158"/>
-      <c r="AN4" s="158"/>
-    </row>
-    <row r="5" spans="1:40" s="68" customFormat="1" ht="65" x14ac:dyDescent="0.2">
-      <c r="A5" s="109" t="s">
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
+      <c r="AM4" s="143"/>
+      <c r="AN4" s="143"/>
+    </row>
+    <row r="5" spans="1:40" s="60" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A5" s="99" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="109" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="113" t="s">
+      <c r="B5" s="99" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="138" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="113" t="s">
+      <c r="E5" s="138" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="113" t="s">
+      <c r="F5" s="138" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="113" t="s">
+      <c r="G5" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="113" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="138" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="168" t="s">
         <v>191</v>
       </c>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="79"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="112" t="s">
-        <v>193</v>
-      </c>
-      <c r="T5" s="112" t="s">
-        <v>194</v>
-      </c>
-      <c r="U5" s="77"/>
-      <c r="V5" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="W5" s="49" t="s">
+      <c r="T5" s="168" t="s">
+        <v>192</v>
+      </c>
+      <c r="U5" s="68"/>
+      <c r="V5" s="136" t="s">
+        <v>191</v>
+      </c>
+      <c r="W5" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="X5" s="49" t="s">
+      <c r="X5" s="136" t="s">
         <v>82</v>
       </c>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="111" t="s">
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="61"/>
+      <c r="AA5" s="202" t="s">
         <v>67</v>
       </c>
-      <c r="AB5" s="111" t="s">
-        <v>190</v>
-      </c>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="49" t="s">
+      <c r="AB5" s="202" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC5" s="134"/>
+      <c r="AD5" s="136" t="s">
         <v>97</v>
       </c>
-      <c r="AE5" s="49"/>
-      <c r="AF5" s="49" t="s">
+      <c r="AE5" s="136"/>
+      <c r="AF5" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AG5" s="49" t="s">
+      <c r="AG5" s="136" t="s">
         <v>79</v>
       </c>
-      <c r="AH5" s="49" t="s">
+      <c r="AH5" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="AI5" s="49" t="s">
+      <c r="AI5" s="136" t="s">
         <v>18</v>
       </c>
-      <c r="AJ5" s="74"/>
-      <c r="AK5" s="19"/>
-      <c r="AL5" s="19"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A6" s="110">
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="64"/>
+      <c r="AL5" s="64"/>
+      <c r="AM5" s="65"/>
+      <c r="AN5" s="65"/>
+    </row>
+    <row r="6" spans="1:40" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="201" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="190"/>
+      <c r="C6" s="197"/>
+      <c r="D6" s="215" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" s="198"/>
+      <c r="F6" s="198"/>
+      <c r="G6" s="198"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="198"/>
+      <c r="J6" s="198"/>
+      <c r="K6" s="198"/>
+      <c r="L6" s="198"/>
+      <c r="M6" s="198"/>
+      <c r="N6" s="198"/>
+      <c r="O6" s="198"/>
+      <c r="P6" s="198"/>
+      <c r="Q6" s="198"/>
+      <c r="R6" s="206"/>
+      <c r="S6" s="180"/>
+      <c r="T6" s="208"/>
+      <c r="U6" s="209"/>
+      <c r="V6" s="210"/>
+      <c r="W6" s="210"/>
+      <c r="X6" s="210"/>
+      <c r="Y6" s="205"/>
+      <c r="Z6" s="211"/>
+      <c r="AA6" s="211"/>
+      <c r="AB6" s="211"/>
+      <c r="AC6" s="209"/>
+      <c r="AD6" s="210"/>
+      <c r="AE6" s="210"/>
+      <c r="AF6" s="210"/>
+      <c r="AG6" s="212"/>
+      <c r="AH6" s="213"/>
+      <c r="AI6" s="213"/>
+      <c r="AJ6" s="214"/>
+      <c r="AK6" s="199"/>
+      <c r="AL6" s="199"/>
+      <c r="AM6" s="200"/>
+      <c r="AN6" s="200"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A7" s="100">
         <v>1</v>
       </c>
-      <c r="AI6" s="13"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="13"/>
-      <c r="AM6" s="13"/>
-      <c r="AN6" s="13"/>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A7" s="110">
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A8" s="100">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A8" s="110">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A9" s="100">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.15">
-      <c r="A9" s="110" t="s">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="A10" s="100" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.15">
+      <c r="AG15" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>